<commit_message>
Úprava podle generátoru skutečnosti
</commit_message>
<xml_diff>
--- a/414_003_T02_PZp_priloha_B.xlsx
+++ b/414_003_T02_PZp_priloha_B.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\Vysoka_skola\Magisterske_studium\2.ročník-ZS\4IT414-Rizeni_projektu\Semestralka\MS-Project-4IT414\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vse-my.sharepoint.com/personal/posm04_vse_cz/Documents/ZS2020/Řízení_projektů/MS Project REPO/MS-Project-4IT414/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C257E4-683B-4B14-A68F-019D29001946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C257E4-683B-4B14-A68F-019D29001946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -865,6 +869,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,13 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,45 +1234,45 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="98.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="98.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="16" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="27" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="37.5703125" style="32" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="37.5546875" style="32" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+    <row r="1" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="49" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="38" t="s">
@@ -1278,7 +1282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1307,7 +1311,7 @@
         <v>7</v>
       </c>
       <c r="J3" s="31"/>
-      <c r="K3" s="47"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="38" t="s">
         <v>14</v>
       </c>
@@ -1315,22 +1319,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="42">
         <f>SUM(C5:C22)</f>
         <v>66</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="42">
         <f t="shared" ref="D4:E4" si="0">SUM(D5:D22)</f>
         <v>97</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="42">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
@@ -1344,7 +1348,7 @@
       </c>
       <c r="H4" s="23">
         <f ca="1">LN(_xlfn.LOGNORM.INV(RAND(),F4,G4))</f>
-        <v>77.149169649348678</v>
+        <v>70.422842360644822</v>
       </c>
       <c r="I4" s="35">
         <f ca="1">ROUND(IF(G4=0,F4,IF(H4&lt;F4,F4,H4)),$M$3)</f>
@@ -1361,20 +1365,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="50">
-        <v>2</v>
-      </c>
-      <c r="D5" s="50">
+      <c r="C5" s="43">
+        <v>2</v>
+      </c>
+      <c r="D5" s="43">
         <v>3</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="43">
         <v>4</v>
       </c>
       <c r="F5" s="1">
@@ -1387,10 +1391,10 @@
       </c>
       <c r="H5" s="23">
         <f t="shared" ref="H5:H58" ca="1" si="3">LN(_xlfn.LOGNORM.INV(RAND(),F5,G5))</f>
-        <v>2.5905777410561828</v>
+        <v>2.2385296815257112</v>
       </c>
       <c r="I5" s="35">
-        <f t="shared" ref="H5:K58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
+        <f t="shared" ref="I5:I58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
         <v>3</v>
       </c>
       <c r="J5" s="28"/>
@@ -1398,20 +1402,20 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="50">
-        <v>2</v>
-      </c>
-      <c r="D6" s="50">
+      <c r="C6" s="43">
+        <v>2</v>
+      </c>
+      <c r="D6" s="43">
         <v>3</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="43">
         <v>4</v>
       </c>
       <c r="F6" s="1">
@@ -1424,31 +1428,31 @@
       </c>
       <c r="H6" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9114747343017386</v>
+        <v>3.3433236013274166</v>
       </c>
       <c r="I6" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.34</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="39">
         <v>3.21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>4</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="43">
         <v>3</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="43">
         <v>4</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="43">
         <v>5</v>
       </c>
       <c r="F7" s="1">
@@ -1461,7 +1465,7 @@
       </c>
       <c r="H7" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0852352723457162</v>
+        <v>3.1731345739695156</v>
       </c>
       <c r="I7" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1472,20 +1476,20 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="43">
         <v>4</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="43">
         <v>5</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="43">
         <v>7</v>
       </c>
       <c r="F8" s="1">
@@ -1498,31 +1502,31 @@
       </c>
       <c r="H8" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2021872523261656</v>
+        <v>5.9406873105250844</v>
       </c>
       <c r="I8" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.94</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>6</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="50">
-        <v>2</v>
-      </c>
-      <c r="D9" s="50">
+      <c r="C9" s="43">
+        <v>2</v>
+      </c>
+      <c r="D9" s="43">
         <v>3</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="43">
         <v>4</v>
       </c>
       <c r="F9" s="1">
@@ -1535,31 +1539,31 @@
       </c>
       <c r="H9" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9257409550891769</v>
+        <v>3.8581638721818448</v>
       </c>
       <c r="I9" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.86</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="39">
         <v>3.18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>7</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="43">
         <v>6</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="43">
         <v>10</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="43">
         <v>14</v>
       </c>
       <c r="F10" s="1">
@@ -1572,31 +1576,31 @@
       </c>
       <c r="H10" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.718913771901137</v>
+        <v>11.919320836288385</v>
       </c>
       <c r="I10" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.72</v>
+        <v>11.92</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="39">
         <v>12.1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="43">
         <v>4</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="43">
         <v>5</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="43">
         <v>5</v>
       </c>
       <c r="F11" s="1">
@@ -1609,31 +1613,31 @@
       </c>
       <c r="H11" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3853748854680283</v>
+        <v>4.8485205624913963</v>
       </c>
       <c r="I11" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.39</v>
+        <v>5</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="50">
+      <c r="C12" s="43">
         <v>1</v>
       </c>
-      <c r="D12" s="50">
-        <v>2</v>
-      </c>
-      <c r="E12" s="50">
+      <c r="D12" s="43">
+        <v>2</v>
+      </c>
+      <c r="E12" s="43">
         <v>3</v>
       </c>
       <c r="F12" s="1">
@@ -1646,31 +1650,31 @@
       </c>
       <c r="H12" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9828523474253772</v>
+        <v>2.2032999825020272</v>
       </c>
       <c r="I12" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="50">
+      <c r="C13" s="43">
         <v>3</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="43">
         <v>4</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="43">
         <v>5</v>
       </c>
       <c r="F13" s="1">
@@ -1683,7 +1687,7 @@
       </c>
       <c r="H13" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1135753207259422</v>
+        <v>3.6151067927017131</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1694,20 +1698,20 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="50">
-        <v>2</v>
-      </c>
-      <c r="D14" s="50">
+      <c r="C14" s="43">
+        <v>2</v>
+      </c>
+      <c r="D14" s="43">
         <v>3</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="43">
         <v>4</v>
       </c>
       <c r="F14" s="1">
@@ -1720,31 +1724,31 @@
       </c>
       <c r="H14" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2176997360846005</v>
+        <v>2.8952890431414282</v>
       </c>
       <c r="I14" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.22</v>
+        <v>3</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="39">
         <v>3.42</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="43">
         <v>6</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="43">
         <v>8</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="43">
         <v>11</v>
       </c>
       <c r="F15" s="1">
@@ -1757,31 +1761,31 @@
       </c>
       <c r="H15" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5408511348571707</v>
+        <v>10.413734169526345</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>10.41</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="39">
         <v>9.26</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="43">
         <v>4</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="43">
         <v>7</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="43">
         <v>10</v>
       </c>
       <c r="F16" s="1">
@@ -1794,31 +1798,31 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5248715608404275</v>
+        <v>8.5382665140384635</v>
       </c>
       <c r="I16" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>8.5399999999999991</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="39">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="43">
         <v>6</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="43">
         <v>10</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="43">
         <v>14</v>
       </c>
       <c r="F17" s="1">
@@ -1831,31 +1835,31 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.316890041642326</v>
+        <v>10.841897658641829</v>
       </c>
       <c r="I17" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.32</v>
+        <v>10.84</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="43">
         <v>3</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="43">
         <v>4</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="43">
         <v>5</v>
       </c>
       <c r="F18" s="1">
@@ -1868,7 +1872,7 @@
       </c>
       <c r="H18" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7389870078287406</v>
+        <v>2.9579656845973119</v>
       </c>
       <c r="I18" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1879,20 +1883,20 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>16</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="50">
+      <c r="C19" s="43">
         <v>6</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="43">
         <v>8</v>
       </c>
-      <c r="E19" s="50">
+      <c r="E19" s="43">
         <v>11</v>
       </c>
       <c r="F19" s="1">
@@ -1905,31 +1909,31 @@
       </c>
       <c r="H19" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.234661405537191</v>
+        <v>9.5445441168162493</v>
       </c>
       <c r="I19" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.23</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="39">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>17</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="43">
         <v>6</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="43">
         <v>10</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="43">
         <v>14</v>
       </c>
       <c r="F20" s="1">
@@ -1942,31 +1946,31 @@
       </c>
       <c r="H20" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.0396488216739179</v>
+        <v>11.936802843920209</v>
       </c>
       <c r="I20" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>11.94</v>
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="43">
         <v>3</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="43">
         <v>4</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="43">
         <v>5</v>
       </c>
       <c r="F21" s="1">
@@ -1979,31 +1983,31 @@
       </c>
       <c r="H21" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3813070765421367</v>
+        <v>5.4872689439713671</v>
       </c>
       <c r="I21" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5.49</v>
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22" s="43">
         <v>3</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="43">
         <v>4</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="43">
         <v>5</v>
       </c>
       <c r="F22" s="1">
@@ -2016,7 +2020,7 @@
       </c>
       <c r="H22" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.90184742779181</v>
+        <v>3.8821535762975046</v>
       </c>
       <c r="I22" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2027,22 +2031,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>20</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="42">
         <f>SUM(C24:C34)</f>
         <v>15</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="42">
         <f t="shared" ref="D23:E23" si="5">SUM(D24:D34)</f>
         <v>26</v>
       </c>
-      <c r="E23" s="49">
+      <c r="E23" s="42">
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
@@ -2056,31 +2060,31 @@
       </c>
       <c r="H23" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>27.821704307587016</v>
+        <v>26.285999565855867</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>27.82</v>
+        <v>27</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="39">
         <v>27.59</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>21</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="50">
+      <c r="C24" s="43">
         <v>3</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="43">
         <v>4</v>
       </c>
-      <c r="E24" s="50">
+      <c r="E24" s="43">
         <v>5</v>
       </c>
       <c r="F24" s="1">
@@ -2093,31 +2097,31 @@
       </c>
       <c r="H24" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8708828097095651</v>
+        <v>3.1058119677774472</v>
       </c>
       <c r="I24" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.87</v>
+        <v>4</v>
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>22</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="50">
+      <c r="C25" s="43">
         <v>1</v>
       </c>
-      <c r="D25" s="50">
-        <v>2</v>
-      </c>
-      <c r="E25" s="50">
+      <c r="D25" s="43">
+        <v>2</v>
+      </c>
+      <c r="E25" s="43">
         <v>3</v>
       </c>
       <c r="F25" s="1">
@@ -2130,31 +2134,31 @@
       </c>
       <c r="H25" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5580234517740843</v>
+        <v>2.6430210142301549</v>
       </c>
       <c r="I25" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.56</v>
+        <v>2.64</v>
       </c>
       <c r="J25" s="28"/>
       <c r="K25" s="39">
         <v>2.86</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>23</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="50">
+      <c r="C26" s="43">
         <v>1</v>
       </c>
-      <c r="D26" s="50">
-        <v>2</v>
-      </c>
-      <c r="E26" s="50">
+      <c r="D26" s="43">
+        <v>2</v>
+      </c>
+      <c r="E26" s="43">
         <v>4</v>
       </c>
       <c r="F26" s="1">
@@ -2167,7 +2171,7 @@
       </c>
       <c r="H26" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5699476409791187</v>
+        <v>1.4269518083778161</v>
       </c>
       <c r="I26" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2178,20 +2182,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>24</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="50">
+      <c r="C27" s="43">
         <v>1</v>
       </c>
-      <c r="D27" s="50">
-        <v>2</v>
-      </c>
-      <c r="E27" s="50">
+      <c r="D27" s="43">
+        <v>2</v>
+      </c>
+      <c r="E27" s="43">
         <v>4</v>
       </c>
       <c r="F27" s="1">
@@ -2204,31 +2208,31 @@
       </c>
       <c r="H27" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6482961409400545</v>
+        <v>1.000739874179851</v>
       </c>
       <c r="I27" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.65</v>
+        <v>2</v>
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="39">
         <v>2.39</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>25</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="50">
+      <c r="C28" s="43">
         <v>1</v>
       </c>
-      <c r="D28" s="50">
-        <v>2</v>
-      </c>
-      <c r="E28" s="50">
+      <c r="D28" s="43">
+        <v>2</v>
+      </c>
+      <c r="E28" s="43">
         <v>3</v>
       </c>
       <c r="F28" s="1">
@@ -2241,7 +2245,7 @@
       </c>
       <c r="H28" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9132933285596767</v>
+        <v>1.7481236010822245</v>
       </c>
       <c r="I28" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2252,20 +2256,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>26</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="50">
+      <c r="C29" s="43">
         <v>3</v>
       </c>
-      <c r="D29" s="50">
+      <c r="D29" s="43">
         <v>4</v>
       </c>
-      <c r="E29" s="50">
+      <c r="E29" s="43">
         <v>5</v>
       </c>
       <c r="F29" s="1">
@@ -2278,7 +2282,7 @@
       </c>
       <c r="H29" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8243691773235975</v>
+        <v>3.5847162020868</v>
       </c>
       <c r="I29" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2289,20 +2293,20 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>27</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="50">
+      <c r="C30" s="43">
         <v>1</v>
       </c>
-      <c r="D30" s="50">
-        <v>2</v>
-      </c>
-      <c r="E30" s="50">
+      <c r="D30" s="43">
+        <v>2</v>
+      </c>
+      <c r="E30" s="43">
         <v>4</v>
       </c>
       <c r="F30" s="1">
@@ -2315,31 +2319,31 @@
       </c>
       <c r="H30" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0345954232236316</v>
+        <v>1.3153247314189658</v>
       </c>
       <c r="I30" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0299999999999998</v>
+        <v>2</v>
       </c>
       <c r="J30" s="28"/>
       <c r="K30" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>28</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="50">
+      <c r="C31" s="43">
         <v>1</v>
       </c>
-      <c r="D31" s="50">
-        <v>2</v>
-      </c>
-      <c r="E31" s="50">
+      <c r="D31" s="43">
+        <v>2</v>
+      </c>
+      <c r="E31" s="43">
         <v>4</v>
       </c>
       <c r="F31" s="1">
@@ -2352,7 +2356,7 @@
       </c>
       <c r="H31" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1385546758098797</v>
+        <v>0.9984696782795448</v>
       </c>
       <c r="I31" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2363,20 +2367,20 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>29</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="50">
+      <c r="C32" s="43">
         <v>1</v>
       </c>
-      <c r="D32" s="50">
-        <v>2</v>
-      </c>
-      <c r="E32" s="50">
+      <c r="D32" s="43">
+        <v>2</v>
+      </c>
+      <c r="E32" s="43">
         <v>4</v>
       </c>
       <c r="F32" s="1">
@@ -2389,7 +2393,7 @@
       </c>
       <c r="H32" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.93345268338986931</v>
+        <v>1.9390513740256159</v>
       </c>
       <c r="I32" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2400,20 +2404,20 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>30</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="50">
+      <c r="C33" s="43">
         <v>1</v>
       </c>
-      <c r="D33" s="50">
-        <v>2</v>
-      </c>
-      <c r="E33" s="50">
+      <c r="D33" s="43">
+        <v>2</v>
+      </c>
+      <c r="E33" s="43">
         <v>3</v>
       </c>
       <c r="F33" s="1">
@@ -2426,31 +2430,31 @@
       </c>
       <c r="H33" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8509747188136898</v>
+        <v>1.8520686978542893</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.85</v>
+        <v>2</v>
       </c>
       <c r="J33" s="28"/>
       <c r="K33" s="39">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>31</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="43">
         <v>1</v>
       </c>
-      <c r="D34" s="50">
-        <v>2</v>
-      </c>
-      <c r="E34" s="50">
+      <c r="D34" s="43">
+        <v>2</v>
+      </c>
+      <c r="E34" s="43">
         <v>3</v>
       </c>
       <c r="F34" s="1">
@@ -2463,33 +2467,33 @@
       </c>
       <c r="H34" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0286524274824602</v>
+        <v>1.7067329337484376</v>
       </c>
       <c r="I34" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.03</v>
+        <v>2</v>
       </c>
       <c r="J34" s="28"/>
       <c r="K34" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>32</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="49">
+      <c r="C35" s="42">
         <f>SUM(C36:C51)</f>
         <v>77</v>
       </c>
-      <c r="D35" s="49">
+      <c r="D35" s="42">
         <f t="shared" ref="D35:E35" si="6">SUM(D36:D51)</f>
         <v>152</v>
       </c>
-      <c r="E35" s="49">
+      <c r="E35" s="42">
         <f t="shared" si="6"/>
         <v>235</v>
       </c>
@@ -2503,31 +2507,31 @@
       </c>
       <c r="H35" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>170.19109632569635</v>
+        <v>170.43316155415087</v>
       </c>
       <c r="I35" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>170.19</v>
+        <v>170.43</v>
       </c>
       <c r="J35" s="28"/>
       <c r="K35" s="39">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>33</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="50">
+      <c r="C36" s="43">
         <v>3</v>
       </c>
-      <c r="D36" s="50">
+      <c r="D36" s="43">
         <v>5</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="43">
         <v>8</v>
       </c>
       <c r="F36" s="1">
@@ -2540,31 +2544,31 @@
       </c>
       <c r="H36" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.1500762632544772</v>
+        <v>6.1548503060607871</v>
       </c>
       <c r="I36" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>6.15</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="39">
         <v>5.21</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>34</v>
       </c>
-      <c r="B37" s="48" t="s">
+      <c r="B37" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="43">
         <v>3</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="43">
         <v>6</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="43">
         <v>10</v>
       </c>
       <c r="F37" s="1">
@@ -2577,31 +2581,31 @@
       </c>
       <c r="H37" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1191999240944099</v>
+        <v>6.8539121994701047</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.12</v>
+        <v>6.85</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="39">
         <v>7.17</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>35</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="50">
+      <c r="C38" s="43">
         <v>15</v>
       </c>
-      <c r="D38" s="50">
+      <c r="D38" s="43">
         <v>35</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="43">
         <v>55</v>
       </c>
       <c r="F38" s="1">
@@ -2614,31 +2618,31 @@
       </c>
       <c r="H38" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>59.434880607771674</v>
+        <v>25.946209206651005</v>
       </c>
       <c r="I38" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>59.43</v>
+        <v>35</v>
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="39">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>36</v>
       </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="50">
+      <c r="C39" s="43">
         <v>3</v>
       </c>
-      <c r="D39" s="50">
+      <c r="D39" s="43">
         <v>5</v>
       </c>
-      <c r="E39" s="50">
+      <c r="E39" s="43">
         <v>8</v>
       </c>
       <c r="F39" s="1">
@@ -2651,31 +2655,31 @@
       </c>
       <c r="H39" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7421726032849261</v>
+        <v>6.0039774870612135</v>
       </c>
       <c r="I39" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.74</v>
+        <v>6</v>
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="39">
         <v>6.09</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>37</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="50">
+      <c r="C40" s="43">
         <v>6</v>
       </c>
-      <c r="D40" s="50">
+      <c r="D40" s="43">
         <v>9</v>
       </c>
-      <c r="E40" s="50">
+      <c r="E40" s="43">
         <v>15</v>
       </c>
       <c r="F40" s="1">
@@ -2688,31 +2692,31 @@
       </c>
       <c r="H40" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5810969944735369</v>
+        <v>10.901929323378592</v>
       </c>
       <c r="I40" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>10.9</v>
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>38</v>
       </c>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="50">
-        <v>2</v>
-      </c>
-      <c r="D41" s="50">
+      <c r="C41" s="43">
+        <v>2</v>
+      </c>
+      <c r="D41" s="43">
         <v>5</v>
       </c>
-      <c r="E41" s="50">
+      <c r="E41" s="43">
         <v>8</v>
       </c>
       <c r="F41" s="1">
@@ -2725,31 +2729,31 @@
       </c>
       <c r="H41" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.7221699751293684</v>
+        <v>4.5673609277607614</v>
       </c>
       <c r="I41" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>7.72</v>
+        <v>5</v>
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>39</v>
       </c>
-      <c r="B42" s="48" t="s">
+      <c r="B42" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="50">
-        <v>2</v>
-      </c>
-      <c r="D42" s="50">
+      <c r="C42" s="43">
+        <v>2</v>
+      </c>
+      <c r="D42" s="43">
         <v>3</v>
       </c>
-      <c r="E42" s="50">
+      <c r="E42" s="43">
         <v>5</v>
       </c>
       <c r="F42" s="1">
@@ -2762,31 +2766,31 @@
       </c>
       <c r="H42" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6607536012778636</v>
+        <v>3.7550439098814459</v>
       </c>
       <c r="I42" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.76</v>
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="39">
         <v>3.16</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>40</v>
       </c>
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="50">
+      <c r="C43" s="43">
         <v>3</v>
       </c>
-      <c r="D43" s="50">
+      <c r="D43" s="43">
         <v>6</v>
       </c>
-      <c r="E43" s="50">
+      <c r="E43" s="43">
         <v>8</v>
       </c>
       <c r="F43" s="1">
@@ -2799,31 +2803,31 @@
       </c>
       <c r="H43" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.6320491664757029</v>
+        <v>9.0876474655128128</v>
       </c>
       <c r="I43" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8.6300000000000008</v>
+        <v>9.09</v>
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="39">
         <v>7.33</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>41</v>
       </c>
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="50">
+      <c r="C44" s="43">
         <v>10</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="43">
         <v>20</v>
       </c>
-      <c r="E44" s="50">
+      <c r="E44" s="43">
         <v>30</v>
       </c>
       <c r="F44" s="1">
@@ -2836,7 +2840,7 @@
       </c>
       <c r="H44" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>13.630711908261214</v>
+        <v>18.02754689239265</v>
       </c>
       <c r="I44" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2847,20 +2851,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>42</v>
       </c>
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="50">
+      <c r="C45" s="43">
         <v>5</v>
       </c>
-      <c r="D45" s="50">
+      <c r="D45" s="43">
         <v>10</v>
       </c>
-      <c r="E45" s="50">
+      <c r="E45" s="43">
         <v>15</v>
       </c>
       <c r="F45" s="1">
@@ -2873,31 +2877,31 @@
       </c>
       <c r="H45" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.302629898425314</v>
+        <v>16.297446973552752</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.3</v>
+        <v>16.3</v>
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="39">
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>43</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="50">
+      <c r="C46" s="43">
         <v>10</v>
       </c>
-      <c r="D46" s="50">
+      <c r="D46" s="43">
         <v>20</v>
       </c>
-      <c r="E46" s="50">
+      <c r="E46" s="43">
         <v>30</v>
       </c>
       <c r="F46" s="1">
@@ -2910,7 +2914,7 @@
       </c>
       <c r="H46" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>19.921031266705697</v>
+        <v>18.816146907096883</v>
       </c>
       <c r="I46" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2921,20 +2925,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>44</v>
       </c>
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="50">
+      <c r="C47" s="43">
         <v>3</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="43">
         <v>5</v>
       </c>
-      <c r="E47" s="50">
+      <c r="E47" s="43">
         <v>8</v>
       </c>
       <c r="F47" s="1">
@@ -2947,7 +2951,7 @@
       </c>
       <c r="H47" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.902438453875118</v>
+        <v>4.4019749230409708</v>
       </c>
       <c r="I47" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2958,20 +2962,20 @@
         <v>5.14</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>45</v>
       </c>
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="50">
+      <c r="C48" s="43">
         <v>1</v>
       </c>
-      <c r="D48" s="50">
-        <v>2</v>
-      </c>
-      <c r="E48" s="50">
+      <c r="D48" s="43">
+        <v>2</v>
+      </c>
+      <c r="E48" s="43">
         <v>3</v>
       </c>
       <c r="F48" s="1">
@@ -2984,31 +2988,31 @@
       </c>
       <c r="H48" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.3271163610881564</v>
+        <v>2.1316192346236189</v>
       </c>
       <c r="I48" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.33</v>
+        <v>2.13</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="39">
         <v>2.15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>46</v>
       </c>
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="50">
+      <c r="C49" s="43">
         <v>1</v>
       </c>
-      <c r="D49" s="50">
+      <c r="D49" s="43">
         <v>1</v>
       </c>
-      <c r="E49" s="50">
+      <c r="E49" s="43">
         <v>2</v>
       </c>
       <c r="F49" s="1">
@@ -3021,7 +3025,7 @@
       </c>
       <c r="H49" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6782906190755108</v>
+        <v>0.79866734165891162</v>
       </c>
       <c r="I49" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3032,20 +3036,20 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>47</v>
       </c>
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="50">
+      <c r="C50" s="43">
         <v>5</v>
       </c>
-      <c r="D50" s="50">
+      <c r="D50" s="43">
         <v>10</v>
       </c>
-      <c r="E50" s="50">
+      <c r="E50" s="43">
         <v>15</v>
       </c>
       <c r="F50" s="1">
@@ -3058,7 +3062,7 @@
       </c>
       <c r="H50" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.0796816318331253</v>
+        <v>9.581165574201183</v>
       </c>
       <c r="I50" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3069,20 +3073,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>48</v>
       </c>
-      <c r="B51" s="48" t="s">
+      <c r="B51" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="50">
+      <c r="C51" s="43">
         <v>5</v>
       </c>
-      <c r="D51" s="50">
+      <c r="D51" s="43">
         <v>10</v>
       </c>
-      <c r="E51" s="50">
+      <c r="E51" s="43">
         <v>15</v>
       </c>
       <c r="F51" s="1">
@@ -3095,33 +3099,33 @@
       </c>
       <c r="H51" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.9873873171284639</v>
+        <v>10.618648514094041</v>
       </c>
       <c r="I51" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>10.62</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>49</v>
       </c>
-      <c r="B52" s="48" t="s">
+      <c r="B52" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="49">
+      <c r="C52" s="42">
         <f>SUM(C53:C58)</f>
         <v>21</v>
       </c>
-      <c r="D52" s="49">
+      <c r="D52" s="42">
         <f t="shared" ref="D52:E52" si="7">SUM(D53:D58)</f>
         <v>29</v>
       </c>
-      <c r="E52" s="49">
+      <c r="E52" s="42">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
@@ -3135,31 +3139,31 @@
       </c>
       <c r="H52" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>33.341819154237271</v>
+        <v>31.4019126084231</v>
       </c>
       <c r="I52" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>33.340000000000003</v>
+        <v>31.4</v>
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="39">
         <v>34.6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>50</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="50">
-        <v>2</v>
-      </c>
-      <c r="D53" s="50">
+      <c r="C53" s="43">
+        <v>2</v>
+      </c>
+      <c r="D53" s="43">
         <v>3</v>
       </c>
-      <c r="E53" s="50">
+      <c r="E53" s="43">
         <v>5</v>
       </c>
       <c r="F53" s="1">
@@ -3172,31 +3176,31 @@
       </c>
       <c r="H53" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1158791945389992</v>
+        <v>2.043829597023834</v>
       </c>
       <c r="I53" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.12</v>
+        <v>3</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="39">
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>51</v>
       </c>
-      <c r="B54" s="48" t="s">
+      <c r="B54" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="50">
+      <c r="C54" s="43">
         <v>1</v>
       </c>
-      <c r="D54" s="50">
+      <c r="D54" s="43">
         <v>1</v>
       </c>
-      <c r="E54" s="50">
+      <c r="E54" s="43">
         <v>2</v>
       </c>
       <c r="F54" s="1">
@@ -3209,31 +3213,31 @@
       </c>
       <c r="H54" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.77707082826872553</v>
+        <v>1.3271837214457838</v>
       </c>
       <c r="I54" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1.33</v>
       </c>
       <c r="J54" s="28"/>
       <c r="K54" s="39">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>52</v>
       </c>
-      <c r="B55" s="48" t="s">
+      <c r="B55" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="50">
+      <c r="C55" s="43">
         <v>1</v>
       </c>
-      <c r="D55" s="50">
-        <v>2</v>
-      </c>
-      <c r="E55" s="50">
+      <c r="D55" s="43">
+        <v>2</v>
+      </c>
+      <c r="E55" s="43">
         <v>3</v>
       </c>
       <c r="F55" s="1">
@@ -3246,31 +3250,31 @@
       </c>
       <c r="H55" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1056702636022044</v>
+        <v>1.7119693639261429</v>
       </c>
       <c r="I55" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.11</v>
+        <v>2</v>
       </c>
       <c r="J55" s="28"/>
       <c r="K55" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>53</v>
       </c>
-      <c r="B56" s="48" t="s">
+      <c r="B56" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="50">
+      <c r="C56" s="43">
         <v>12</v>
       </c>
-      <c r="D56" s="50">
+      <c r="D56" s="43">
         <v>15</v>
       </c>
-      <c r="E56" s="50">
+      <c r="E56" s="43">
         <v>17</v>
       </c>
       <c r="F56" s="1">
@@ -3283,7 +3287,7 @@
       </c>
       <c r="H56" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>14.541766659713996</v>
+        <v>14.718247474174472</v>
       </c>
       <c r="I56" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3294,20 +3298,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>54</v>
       </c>
-      <c r="B57" s="48" t="s">
+      <c r="B57" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="50">
+      <c r="C57" s="43">
         <v>3</v>
       </c>
-      <c r="D57" s="50">
+      <c r="D57" s="43">
         <v>5</v>
       </c>
-      <c r="E57" s="50">
+      <c r="E57" s="43">
         <v>8</v>
       </c>
       <c r="F57" s="1">
@@ -3320,31 +3324,31 @@
       </c>
       <c r="H57" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3248421810813156</v>
+        <v>5.3860028232022712</v>
       </c>
       <c r="I57" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.39</v>
       </c>
       <c r="J57" s="28"/>
       <c r="K57" s="39">
         <v>7.27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>55</v>
       </c>
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="50">
-        <v>2</v>
-      </c>
-      <c r="D58" s="50">
+      <c r="C58" s="43">
+        <v>2</v>
+      </c>
+      <c r="D58" s="43">
         <v>3</v>
       </c>
-      <c r="E58" s="50">
+      <c r="E58" s="43">
         <v>5</v>
       </c>
       <c r="F58" s="1">
@@ -3357,18 +3361,18 @@
       </c>
       <c r="H58" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3184840739195023</v>
+        <v>3.4348613356450941</v>
       </c>
       <c r="I58" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.32</v>
+        <v>3.43</v>
       </c>
       <c r="J58" s="28"/>
       <c r="K58" s="39">
         <v>3.97</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="F59" s="2"/>
       <c r="G59" s="5"/>
@@ -3377,7 +3381,7 @@
       <c r="J59" s="28"/>
       <c r="K59" s="39"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -3390,7 +3394,7 @@
       <c r="J60" s="28"/>
       <c r="K60" s="39"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -3403,7 +3407,7 @@
       <c r="J61" s="28"/>
       <c r="K61" s="39"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
@@ -3416,7 +3420,7 @@
       <c r="J62" s="28"/>
       <c r="K62" s="39"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
@@ -3429,7 +3433,7 @@
       <c r="J63" s="28"/>
       <c r="K63" s="39"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
@@ -3442,7 +3446,7 @@
       <c r="J64" s="28"/>
       <c r="K64" s="39"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
@@ -3455,7 +3459,7 @@
       <c r="J65" s="28"/>
       <c r="K65" s="39"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
@@ -3468,7 +3472,7 @@
       <c r="J66" s="28"/>
       <c r="K66" s="39"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
@@ -3481,7 +3485,7 @@
       <c r="J67" s="28"/>
       <c r="K67" s="39"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
@@ -3494,7 +3498,7 @@
       <c r="J68" s="28"/>
       <c r="K68" s="39"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
@@ -3507,7 +3511,7 @@
       <c r="J69" s="28"/>
       <c r="K69" s="39"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
@@ -3520,7 +3524,7 @@
       <c r="J70" s="28"/>
       <c r="K70" s="39"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
@@ -3533,7 +3537,7 @@
       <c r="J71" s="28"/>
       <c r="K71" s="39"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="19"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
@@ -3546,7 +3550,7 @@
       <c r="J72" s="28"/>
       <c r="K72" s="39"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -3559,7 +3563,7 @@
       <c r="J73" s="28"/>
       <c r="K73" s="39"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
@@ -3572,7 +3576,7 @@
       <c r="J74" s="28"/>
       <c r="K74" s="39"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -3585,7 +3589,7 @@
       <c r="J75" s="28"/>
       <c r="K75" s="39"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -3598,7 +3602,7 @@
       <c r="J76" s="28"/>
       <c r="K76" s="39"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -3611,7 +3615,7 @@
       <c r="J77" s="28"/>
       <c r="K77" s="39"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -3624,7 +3628,7 @@
       <c r="J78" s="28"/>
       <c r="K78" s="39"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -3637,7 +3641,7 @@
       <c r="J79" s="28"/>
       <c r="K79" s="39"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -3650,7 +3654,7 @@
       <c r="J80" s="28"/>
       <c r="K80" s="39"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3663,7 +3667,7 @@
       <c r="J81" s="28"/>
       <c r="K81" s="39"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3676,7 +3680,7 @@
       <c r="J82" s="28"/>
       <c r="K82" s="39"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3689,7 +3693,7 @@
       <c r="J83" s="28"/>
       <c r="K83" s="39"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3702,7 +3706,7 @@
       <c r="J84" s="28"/>
       <c r="K84" s="39"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="19"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3715,7 +3719,7 @@
       <c r="J85" s="28"/>
       <c r="K85" s="39"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="19"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3728,7 +3732,7 @@
       <c r="J86" s="28"/>
       <c r="K86" s="39"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="19"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -3741,7 +3745,7 @@
       <c r="J87" s="28"/>
       <c r="K87" s="39"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -3754,7 +3758,7 @@
       <c r="J88" s="28"/>
       <c r="K88" s="39"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="19"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -3767,7 +3771,7 @@
       <c r="J89" s="28"/>
       <c r="K89" s="39"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="19"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -3780,7 +3784,7 @@
       <c r="J90" s="28"/>
       <c r="K90" s="39"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="19"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
@@ -3793,7 +3797,7 @@
       <c r="J91" s="28"/>
       <c r="K91" s="39"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="19"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
@@ -3806,7 +3810,7 @@
       <c r="J92" s="28"/>
       <c r="K92" s="39"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="19"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
@@ -3819,7 +3823,7 @@
       <c r="J93" s="28"/>
       <c r="K93" s="39"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="19"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
@@ -3832,7 +3836,7 @@
       <c r="J94" s="28"/>
       <c r="K94" s="39"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="19"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
@@ -3845,7 +3849,7 @@
       <c r="J95" s="28"/>
       <c r="K95" s="39"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="19"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
@@ -3858,7 +3862,7 @@
       <c r="J96" s="28"/>
       <c r="K96" s="39"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="19"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
@@ -3871,7 +3875,7 @@
       <c r="J97" s="28"/>
       <c r="K97" s="39"/>
     </row>
-    <row r="98" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="10"/>
       <c r="C98" s="11"/>
@@ -3908,7 +3912,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -3922,7 +3926,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>

<commit_message>
Revert "Úprava podle generátoru skutečnosti"
This reverts commit 8207c787b43cb630bed1a7e7a8924ab46dca55c1.
</commit_message>
<xml_diff>
--- a/414_003_T02_PZp_priloha_B.xlsx
+++ b/414_003_T02_PZp_priloha_B.xlsx
@@ -1,31 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vse-my.sharepoint.com/personal/posm04_vse_cz/Documents/ZS2020/Řízení_projektů/MS Project REPO/MS-Project-4IT414/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\Vysoka_skola\Magisterske_studium\2.ročník-ZS\4IT414-Rizeni_projektu\Semestralka\MS-Project-4IT414\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C257E4-683B-4B14-A68F-019D29001946}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C257E4-683B-4B14-A68F-019D29001946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -869,13 +865,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -892,6 +881,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1234,45 +1230,45 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="98.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="98.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="16" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" style="27" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.5546875" style="32" customWidth="1"/>
-    <col min="13" max="14" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="27" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="37.5703125" style="32" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="49" t="s">
+      <c r="K2" s="46" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="38" t="s">
@@ -1282,7 +1278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1311,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="J3" s="31"/>
-      <c r="K3" s="50"/>
+      <c r="K3" s="47"/>
       <c r="L3" s="38" t="s">
         <v>14</v>
       </c>
@@ -1319,22 +1315,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="49">
         <f>SUM(C5:C22)</f>
         <v>66</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="49">
         <f t="shared" ref="D4:E4" si="0">SUM(D5:D22)</f>
         <v>97</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="49">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
@@ -1348,7 +1344,7 @@
       </c>
       <c r="H4" s="23">
         <f ca="1">LN(_xlfn.LOGNORM.INV(RAND(),F4,G4))</f>
-        <v>70.422842360644822</v>
+        <v>77.149169649348678</v>
       </c>
       <c r="I4" s="35">
         <f ca="1">ROUND(IF(G4=0,F4,IF(H4&lt;F4,F4,H4)),$M$3)</f>
@@ -1365,20 +1361,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="43">
-        <v>2</v>
-      </c>
-      <c r="D5" s="43">
+      <c r="C5" s="50">
+        <v>2</v>
+      </c>
+      <c r="D5" s="50">
         <v>3</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="50">
         <v>4</v>
       </c>
       <c r="F5" s="1">
@@ -1391,10 +1387,10 @@
       </c>
       <c r="H5" s="23">
         <f t="shared" ref="H5:H58" ca="1" si="3">LN(_xlfn.LOGNORM.INV(RAND(),F5,G5))</f>
-        <v>2.2385296815257112</v>
+        <v>2.5905777410561828</v>
       </c>
       <c r="I5" s="35">
-        <f t="shared" ref="I5:I58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
+        <f t="shared" ref="H5:K58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
         <v>3</v>
       </c>
       <c r="J5" s="28"/>
@@ -1402,20 +1398,20 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="43">
-        <v>2</v>
-      </c>
-      <c r="D6" s="43">
+      <c r="C6" s="50">
+        <v>2</v>
+      </c>
+      <c r="D6" s="50">
         <v>3</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="50">
         <v>4</v>
       </c>
       <c r="F6" s="1">
@@ -1428,31 +1424,31 @@
       </c>
       <c r="H6" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3433236013274166</v>
+        <v>2.9114747343017386</v>
       </c>
       <c r="I6" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.34</v>
+        <v>3</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="39">
         <v>3.21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>4</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="50">
         <v>3</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="50">
         <v>4</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="50">
         <v>5</v>
       </c>
       <c r="F7" s="1">
@@ -1465,7 +1461,7 @@
       </c>
       <c r="H7" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1731345739695156</v>
+        <v>3.0852352723457162</v>
       </c>
       <c r="I7" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1476,20 +1472,20 @@
         <v>4.87</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="50">
         <v>4</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="50">
         <v>5</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="50">
         <v>7</v>
       </c>
       <c r="F8" s="1">
@@ -1502,31 +1498,31 @@
       </c>
       <c r="H8" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.9406873105250844</v>
+        <v>4.2021872523261656</v>
       </c>
       <c r="I8" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.94</v>
+        <v>5</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>6</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="43">
-        <v>2</v>
-      </c>
-      <c r="D9" s="43">
+      <c r="C9" s="50">
+        <v>2</v>
+      </c>
+      <c r="D9" s="50">
         <v>3</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="50">
         <v>4</v>
       </c>
       <c r="F9" s="1">
@@ -1539,31 +1535,31 @@
       </c>
       <c r="H9" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8581638721818448</v>
+        <v>2.9257409550891769</v>
       </c>
       <c r="I9" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.86</v>
+        <v>3</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="39">
         <v>3.18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>7</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="50">
         <v>6</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="50">
         <v>10</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="50">
         <v>14</v>
       </c>
       <c r="F10" s="1">
@@ -1576,31 +1572,31 @@
       </c>
       <c r="H10" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.919320836288385</v>
+        <v>10.718913771901137</v>
       </c>
       <c r="I10" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.92</v>
+        <v>10.72</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="39">
         <v>12.1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="50">
         <v>4</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="50">
         <v>5</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="50">
         <v>5</v>
       </c>
       <c r="F11" s="1">
@@ -1613,31 +1609,31 @@
       </c>
       <c r="H11" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8485205624913963</v>
+        <v>5.3853748854680283</v>
       </c>
       <c r="I11" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.39</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="50">
         <v>1</v>
       </c>
-      <c r="D12" s="43">
-        <v>2</v>
-      </c>
-      <c r="E12" s="43">
+      <c r="D12" s="50">
+        <v>2</v>
+      </c>
+      <c r="E12" s="50">
         <v>3</v>
       </c>
       <c r="F12" s="1">
@@ -1650,31 +1646,31 @@
       </c>
       <c r="H12" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.2032999825020272</v>
+        <v>1.9828523474253772</v>
       </c>
       <c r="I12" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="50">
         <v>3</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="50">
         <v>4</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="50">
         <v>5</v>
       </c>
       <c r="F13" s="1">
@@ -1687,7 +1683,7 @@
       </c>
       <c r="H13" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.6151067927017131</v>
+        <v>3.1135753207259422</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1698,20 +1694,20 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="43">
-        <v>2</v>
-      </c>
-      <c r="D14" s="43">
+      <c r="C14" s="50">
+        <v>2</v>
+      </c>
+      <c r="D14" s="50">
         <v>3</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="50">
         <v>4</v>
       </c>
       <c r="F14" s="1">
@@ -1724,31 +1720,31 @@
       </c>
       <c r="H14" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8952890431414282</v>
+        <v>3.2176997360846005</v>
       </c>
       <c r="I14" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.22</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="39">
         <v>3.42</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="50">
         <v>6</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="50">
         <v>8</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="50">
         <v>11</v>
       </c>
       <c r="F15" s="1">
@@ -1761,31 +1757,31 @@
       </c>
       <c r="H15" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.413734169526345</v>
+        <v>7.5408511348571707</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.41</v>
+        <v>8</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="39">
         <v>9.26</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="50">
         <v>4</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="50">
         <v>7</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="50">
         <v>10</v>
       </c>
       <c r="F16" s="1">
@@ -1798,31 +1794,31 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.5382665140384635</v>
+        <v>5.5248715608404275</v>
       </c>
       <c r="I16" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8.5399999999999991</v>
+        <v>7</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="39">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="50">
         <v>6</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="50">
         <v>10</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="50">
         <v>14</v>
       </c>
       <c r="F17" s="1">
@@ -1835,31 +1831,31 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.841897658641829</v>
+        <v>11.316890041642326</v>
       </c>
       <c r="I17" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.84</v>
+        <v>11.32</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="50">
         <v>3</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="50">
         <v>4</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="50">
         <v>5</v>
       </c>
       <c r="F18" s="1">
@@ -1872,7 +1868,7 @@
       </c>
       <c r="H18" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9579656845973119</v>
+        <v>3.7389870078287406</v>
       </c>
       <c r="I18" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1883,20 +1879,20 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>16</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="50">
         <v>6</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="50">
         <v>8</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="50">
         <v>11</v>
       </c>
       <c r="F19" s="1">
@@ -1909,31 +1905,31 @@
       </c>
       <c r="H19" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.5445441168162493</v>
+        <v>10.234661405537191</v>
       </c>
       <c r="I19" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>9.5399999999999991</v>
+        <v>10.23</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="39">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>17</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="50">
         <v>6</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="50">
         <v>10</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="50">
         <v>14</v>
       </c>
       <c r="F20" s="1">
@@ -1946,31 +1942,31 @@
       </c>
       <c r="H20" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.936802843920209</v>
+        <v>8.0396488216739179</v>
       </c>
       <c r="I20" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.94</v>
+        <v>10</v>
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="50">
         <v>3</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="50">
         <v>4</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="50">
         <v>5</v>
       </c>
       <c r="F21" s="1">
@@ -1983,31 +1979,31 @@
       </c>
       <c r="H21" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.4872689439713671</v>
+        <v>3.3813070765421367</v>
       </c>
       <c r="I21" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.49</v>
+        <v>4</v>
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="50">
         <v>3</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="50">
         <v>4</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="50">
         <v>5</v>
       </c>
       <c r="F22" s="1">
@@ -2020,7 +2016,7 @@
       </c>
       <c r="H22" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8821535762975046</v>
+        <v>3.90184742779181</v>
       </c>
       <c r="I22" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2031,22 +2027,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>20</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="49">
         <f>SUM(C24:C34)</f>
         <v>15</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="49">
         <f t="shared" ref="D23:E23" si="5">SUM(D24:D34)</f>
         <v>26</v>
       </c>
-      <c r="E23" s="42">
+      <c r="E23" s="49">
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
@@ -2060,31 +2056,31 @@
       </c>
       <c r="H23" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>26.285999565855867</v>
+        <v>27.821704307587016</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>27</v>
+        <v>27.82</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="39">
         <v>27.59</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>21</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="50">
         <v>3</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="50">
         <v>4</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="50">
         <v>5</v>
       </c>
       <c r="F24" s="1">
@@ -2097,31 +2093,31 @@
       </c>
       <c r="H24" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1058119677774472</v>
+        <v>4.8708828097095651</v>
       </c>
       <c r="I24" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.87</v>
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>22</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="50">
         <v>1</v>
       </c>
-      <c r="D25" s="43">
-        <v>2</v>
-      </c>
-      <c r="E25" s="43">
+      <c r="D25" s="50">
+        <v>2</v>
+      </c>
+      <c r="E25" s="50">
         <v>3</v>
       </c>
       <c r="F25" s="1">
@@ -2134,31 +2130,31 @@
       </c>
       <c r="H25" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6430210142301549</v>
+        <v>2.5580234517740843</v>
       </c>
       <c r="I25" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.64</v>
+        <v>2.56</v>
       </c>
       <c r="J25" s="28"/>
       <c r="K25" s="39">
         <v>2.86</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>23</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="50">
         <v>1</v>
       </c>
-      <c r="D26" s="43">
-        <v>2</v>
-      </c>
-      <c r="E26" s="43">
+      <c r="D26" s="50">
+        <v>2</v>
+      </c>
+      <c r="E26" s="50">
         <v>4</v>
       </c>
       <c r="F26" s="1">
@@ -2171,7 +2167,7 @@
       </c>
       <c r="H26" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4269518083778161</v>
+        <v>1.5699476409791187</v>
       </c>
       <c r="I26" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2182,20 +2178,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>24</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="50">
         <v>1</v>
       </c>
-      <c r="D27" s="43">
-        <v>2</v>
-      </c>
-      <c r="E27" s="43">
+      <c r="D27" s="50">
+        <v>2</v>
+      </c>
+      <c r="E27" s="50">
         <v>4</v>
       </c>
       <c r="F27" s="1">
@@ -2208,31 +2204,31 @@
       </c>
       <c r="H27" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.000739874179851</v>
+        <v>2.6482961409400545</v>
       </c>
       <c r="I27" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.65</v>
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="39">
         <v>2.39</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>25</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="50">
         <v>1</v>
       </c>
-      <c r="D28" s="43">
-        <v>2</v>
-      </c>
-      <c r="E28" s="43">
+      <c r="D28" s="50">
+        <v>2</v>
+      </c>
+      <c r="E28" s="50">
         <v>3</v>
       </c>
       <c r="F28" s="1">
@@ -2245,7 +2241,7 @@
       </c>
       <c r="H28" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7481236010822245</v>
+        <v>1.9132933285596767</v>
       </c>
       <c r="I28" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2256,20 +2252,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
         <v>26</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="50">
         <v>3</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="50">
         <v>4</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="50">
         <v>5</v>
       </c>
       <c r="F29" s="1">
@@ -2282,7 +2278,7 @@
       </c>
       <c r="H29" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.5847162020868</v>
+        <v>3.8243691773235975</v>
       </c>
       <c r="I29" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2293,20 +2289,20 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>27</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="50">
         <v>1</v>
       </c>
-      <c r="D30" s="43">
-        <v>2</v>
-      </c>
-      <c r="E30" s="43">
+      <c r="D30" s="50">
+        <v>2</v>
+      </c>
+      <c r="E30" s="50">
         <v>4</v>
       </c>
       <c r="F30" s="1">
@@ -2319,31 +2315,31 @@
       </c>
       <c r="H30" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3153247314189658</v>
+        <v>2.0345954232236316</v>
       </c>
       <c r="I30" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="J30" s="28"/>
       <c r="K30" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>28</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="50">
         <v>1</v>
       </c>
-      <c r="D31" s="43">
-        <v>2</v>
-      </c>
-      <c r="E31" s="43">
+      <c r="D31" s="50">
+        <v>2</v>
+      </c>
+      <c r="E31" s="50">
         <v>4</v>
       </c>
       <c r="F31" s="1">
@@ -2356,7 +2352,7 @@
       </c>
       <c r="H31" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.9984696782795448</v>
+        <v>1.1385546758098797</v>
       </c>
       <c r="I31" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2367,20 +2363,20 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
         <v>29</v>
       </c>
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="50">
         <v>1</v>
       </c>
-      <c r="D32" s="43">
-        <v>2</v>
-      </c>
-      <c r="E32" s="43">
+      <c r="D32" s="50">
+        <v>2</v>
+      </c>
+      <c r="E32" s="50">
         <v>4</v>
       </c>
       <c r="F32" s="1">
@@ -2393,7 +2389,7 @@
       </c>
       <c r="H32" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9390513740256159</v>
+        <v>0.93345268338986931</v>
       </c>
       <c r="I32" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2404,20 +2400,20 @@
         <v>2.41</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
         <v>30</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="50">
         <v>1</v>
       </c>
-      <c r="D33" s="43">
-        <v>2</v>
-      </c>
-      <c r="E33" s="43">
+      <c r="D33" s="50">
+        <v>2</v>
+      </c>
+      <c r="E33" s="50">
         <v>3</v>
       </c>
       <c r="F33" s="1">
@@ -2430,31 +2426,31 @@
       </c>
       <c r="H33" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8520686978542893</v>
+        <v>2.8509747188136898</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.85</v>
       </c>
       <c r="J33" s="28"/>
       <c r="K33" s="39">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>31</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="50">
         <v>1</v>
       </c>
-      <c r="D34" s="43">
-        <v>2</v>
-      </c>
-      <c r="E34" s="43">
+      <c r="D34" s="50">
+        <v>2</v>
+      </c>
+      <c r="E34" s="50">
         <v>3</v>
       </c>
       <c r="F34" s="1">
@@ -2467,33 +2463,33 @@
       </c>
       <c r="H34" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7067329337484376</v>
+        <v>3.0286524274824602</v>
       </c>
       <c r="I34" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3.03</v>
       </c>
       <c r="J34" s="28"/>
       <c r="K34" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
         <v>32</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="49">
         <f>SUM(C36:C51)</f>
         <v>77</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="49">
         <f t="shared" ref="D35:E35" si="6">SUM(D36:D51)</f>
         <v>152</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="49">
         <f t="shared" si="6"/>
         <v>235</v>
       </c>
@@ -2507,31 +2503,31 @@
       </c>
       <c r="H35" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>170.43316155415087</v>
+        <v>170.19109632569635</v>
       </c>
       <c r="I35" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>170.43</v>
+        <v>170.19</v>
       </c>
       <c r="J35" s="28"/>
       <c r="K35" s="39">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
         <v>33</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="50">
         <v>3</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D36" s="50">
         <v>5</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="50">
         <v>8</v>
       </c>
       <c r="F36" s="1">
@@ -2544,31 +2540,31 @@
       </c>
       <c r="H36" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1548503060607871</v>
+        <v>4.1500762632544772</v>
       </c>
       <c r="I36" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.15</v>
+        <v>5</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="39">
         <v>5.21</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
         <v>34</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="50">
         <v>3</v>
       </c>
-      <c r="D37" s="43">
+      <c r="D37" s="50">
         <v>6</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="50">
         <v>10</v>
       </c>
       <c r="F37" s="1">
@@ -2581,31 +2577,31 @@
       </c>
       <c r="H37" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.8539121994701047</v>
+        <v>6.1191999240944099</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.85</v>
+        <v>6.12</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="39">
         <v>7.17</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
         <v>35</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="50">
         <v>15</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="50">
         <v>35</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="50">
         <v>55</v>
       </c>
       <c r="F38" s="1">
@@ -2618,31 +2614,31 @@
       </c>
       <c r="H38" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>25.946209206651005</v>
+        <v>59.434880607771674</v>
       </c>
       <c r="I38" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>35</v>
+        <v>59.43</v>
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="39">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>36</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="50">
         <v>3</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="50">
         <v>5</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="50">
         <v>8</v>
       </c>
       <c r="F39" s="1">
@@ -2655,31 +2651,31 @@
       </c>
       <c r="H39" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.0039774870612135</v>
+        <v>5.7421726032849261</v>
       </c>
       <c r="I39" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5.74</v>
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="39">
         <v>6.09</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
         <v>37</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="50">
         <v>6</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D40" s="50">
         <v>9</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="50">
         <v>15</v>
       </c>
       <c r="F40" s="1">
@@ -2692,31 +2688,31 @@
       </c>
       <c r="H40" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.901929323378592</v>
+        <v>7.5810969944735369</v>
       </c>
       <c r="I40" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.9</v>
+        <v>10</v>
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>38</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="43">
-        <v>2</v>
-      </c>
-      <c r="D41" s="43">
+      <c r="C41" s="50">
+        <v>2</v>
+      </c>
+      <c r="D41" s="50">
         <v>5</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="50">
         <v>8</v>
       </c>
       <c r="F41" s="1">
@@ -2729,31 +2725,31 @@
       </c>
       <c r="H41" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5673609277607614</v>
+        <v>7.7221699751293684</v>
       </c>
       <c r="I41" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>7.72</v>
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19">
         <v>39</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="43">
-        <v>2</v>
-      </c>
-      <c r="D42" s="43">
+      <c r="C42" s="50">
+        <v>2</v>
+      </c>
+      <c r="D42" s="50">
         <v>3</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="50">
         <v>5</v>
       </c>
       <c r="F42" s="1">
@@ -2766,31 +2762,31 @@
       </c>
       <c r="H42" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7550439098814459</v>
+        <v>2.6607536012778636</v>
       </c>
       <c r="I42" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.76</v>
+        <v>3</v>
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="39">
         <v>3.16</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19">
         <v>40</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="50">
         <v>3</v>
       </c>
-      <c r="D43" s="43">
+      <c r="D43" s="50">
         <v>6</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="50">
         <v>8</v>
       </c>
       <c r="F43" s="1">
@@ -2803,31 +2799,31 @@
       </c>
       <c r="H43" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.0876474655128128</v>
+        <v>8.6320491664757029</v>
       </c>
       <c r="I43" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>9.09</v>
+        <v>8.6300000000000008</v>
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="39">
         <v>7.33</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="19">
         <v>41</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="50">
         <v>10</v>
       </c>
-      <c r="D44" s="43">
+      <c r="D44" s="50">
         <v>20</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="50">
         <v>30</v>
       </c>
       <c r="F44" s="1">
@@ -2840,7 +2836,7 @@
       </c>
       <c r="H44" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>18.02754689239265</v>
+        <v>13.630711908261214</v>
       </c>
       <c r="I44" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2851,20 +2847,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19">
         <v>42</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="50">
         <v>5</v>
       </c>
-      <c r="D45" s="43">
+      <c r="D45" s="50">
         <v>10</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="50">
         <v>15</v>
       </c>
       <c r="F45" s="1">
@@ -2877,31 +2873,31 @@
       </c>
       <c r="H45" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>16.297446973552752</v>
+        <v>11.302629898425314</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>16.3</v>
+        <v>11.3</v>
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="39">
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19">
         <v>43</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="50">
         <v>10</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="50">
         <v>20</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="50">
         <v>30</v>
       </c>
       <c r="F46" s="1">
@@ -2914,7 +2910,7 @@
       </c>
       <c r="H46" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>18.816146907096883</v>
+        <v>19.921031266705697</v>
       </c>
       <c r="I46" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2925,20 +2921,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
         <v>44</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="50">
         <v>3</v>
       </c>
-      <c r="D47" s="43">
+      <c r="D47" s="50">
         <v>5</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="50">
         <v>8</v>
       </c>
       <c r="F47" s="1">
@@ -2951,7 +2947,7 @@
       </c>
       <c r="H47" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.4019749230409708</v>
+        <v>4.902438453875118</v>
       </c>
       <c r="I47" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2962,20 +2958,20 @@
         <v>5.14</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
         <v>45</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="50">
         <v>1</v>
       </c>
-      <c r="D48" s="43">
-        <v>2</v>
-      </c>
-      <c r="E48" s="43">
+      <c r="D48" s="50">
+        <v>2</v>
+      </c>
+      <c r="E48" s="50">
         <v>3</v>
       </c>
       <c r="F48" s="1">
@@ -2988,31 +2984,31 @@
       </c>
       <c r="H48" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1316192346236189</v>
+        <v>2.3271163610881564</v>
       </c>
       <c r="I48" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.13</v>
+        <v>2.33</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="39">
         <v>2.15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
         <v>46</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="50">
         <v>1</v>
       </c>
-      <c r="D49" s="43">
+      <c r="D49" s="50">
         <v>1</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="50">
         <v>2</v>
       </c>
       <c r="F49" s="1">
@@ -3025,7 +3021,7 @@
       </c>
       <c r="H49" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.79866734165891162</v>
+        <v>0.6782906190755108</v>
       </c>
       <c r="I49" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3036,20 +3032,20 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="19">
         <v>47</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="50">
         <v>5</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="50">
         <v>10</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="50">
         <v>15</v>
       </c>
       <c r="F50" s="1">
@@ -3062,7 +3058,7 @@
       </c>
       <c r="H50" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.581165574201183</v>
+        <v>7.0796816318331253</v>
       </c>
       <c r="I50" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3073,20 +3069,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
         <v>48</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="50">
         <v>5</v>
       </c>
-      <c r="D51" s="43">
+      <c r="D51" s="50">
         <v>10</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="50">
         <v>15</v>
       </c>
       <c r="F51" s="1">
@@ -3099,33 +3095,33 @@
       </c>
       <c r="H51" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.618648514094041</v>
+        <v>9.9873873171284639</v>
       </c>
       <c r="I51" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.62</v>
+        <v>10</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19">
         <v>49</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="42">
+      <c r="C52" s="49">
         <f>SUM(C53:C58)</f>
         <v>21</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="49">
         <f t="shared" ref="D52:E52" si="7">SUM(D53:D58)</f>
         <v>29</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="49">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
@@ -3139,31 +3135,31 @@
       </c>
       <c r="H52" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>31.4019126084231</v>
+        <v>33.341819154237271</v>
       </c>
       <c r="I52" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>31.4</v>
+        <v>33.340000000000003</v>
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="39">
         <v>34.6</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>50</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="43">
-        <v>2</v>
-      </c>
-      <c r="D53" s="43">
+      <c r="C53" s="50">
+        <v>2</v>
+      </c>
+      <c r="D53" s="50">
         <v>3</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="50">
         <v>5</v>
       </c>
       <c r="F53" s="1">
@@ -3176,31 +3172,31 @@
       </c>
       <c r="H53" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.043829597023834</v>
+        <v>3.1158791945389992</v>
       </c>
       <c r="I53" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.12</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="39">
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
         <v>51</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="50">
         <v>1</v>
       </c>
-      <c r="D54" s="43">
+      <c r="D54" s="50">
         <v>1</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="50">
         <v>2</v>
       </c>
       <c r="F54" s="1">
@@ -3213,31 +3209,31 @@
       </c>
       <c r="H54" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3271837214457838</v>
+        <v>0.77707082826872553</v>
       </c>
       <c r="I54" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>1.33</v>
+        <v>1</v>
       </c>
       <c r="J54" s="28"/>
       <c r="K54" s="39">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
         <v>52</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="50">
         <v>1</v>
       </c>
-      <c r="D55" s="43">
-        <v>2</v>
-      </c>
-      <c r="E55" s="43">
+      <c r="D55" s="50">
+        <v>2</v>
+      </c>
+      <c r="E55" s="50">
         <v>3</v>
       </c>
       <c r="F55" s="1">
@@ -3250,31 +3246,31 @@
       </c>
       <c r="H55" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.7119693639261429</v>
+        <v>2.1056702636022044</v>
       </c>
       <c r="I55" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.11</v>
       </c>
       <c r="J55" s="28"/>
       <c r="K55" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="19">
         <v>53</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="50">
         <v>12</v>
       </c>
-      <c r="D56" s="43">
+      <c r="D56" s="50">
         <v>15</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="50">
         <v>17</v>
       </c>
       <c r="F56" s="1">
@@ -3287,7 +3283,7 @@
       </c>
       <c r="H56" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>14.718247474174472</v>
+        <v>14.541766659713996</v>
       </c>
       <c r="I56" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -3298,20 +3294,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>54</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="50">
         <v>3</v>
       </c>
-      <c r="D57" s="43">
+      <c r="D57" s="50">
         <v>5</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="50">
         <v>8</v>
       </c>
       <c r="F57" s="1">
@@ -3324,31 +3320,31 @@
       </c>
       <c r="H57" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3860028232022712</v>
+        <v>4.3248421810813156</v>
       </c>
       <c r="I57" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.39</v>
+        <v>5</v>
       </c>
       <c r="J57" s="28"/>
       <c r="K57" s="39">
         <v>7.27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
         <v>55</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="43">
-        <v>2</v>
-      </c>
-      <c r="D58" s="43">
+      <c r="C58" s="50">
+        <v>2</v>
+      </c>
+      <c r="D58" s="50">
         <v>3</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="50">
         <v>5</v>
       </c>
       <c r="F58" s="1">
@@ -3361,18 +3357,18 @@
       </c>
       <c r="H58" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4348613356450941</v>
+        <v>3.3184840739195023</v>
       </c>
       <c r="I58" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.43</v>
+        <v>3.32</v>
       </c>
       <c r="J58" s="28"/>
       <c r="K58" s="39">
         <v>3.97</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="19"/>
       <c r="F59" s="2"/>
       <c r="G59" s="5"/>
@@ -3381,7 +3377,7 @@
       <c r="J59" s="28"/>
       <c r="K59" s="39"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="19"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -3394,7 +3390,7 @@
       <c r="J60" s="28"/>
       <c r="K60" s="39"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -3407,7 +3403,7 @@
       <c r="J61" s="28"/>
       <c r="K61" s="39"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="19"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
@@ -3420,7 +3416,7 @@
       <c r="J62" s="28"/>
       <c r="K62" s="39"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
@@ -3433,7 +3429,7 @@
       <c r="J63" s="28"/>
       <c r="K63" s="39"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
@@ -3446,7 +3442,7 @@
       <c r="J64" s="28"/>
       <c r="K64" s="39"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
@@ -3459,7 +3455,7 @@
       <c r="J65" s="28"/>
       <c r="K65" s="39"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="19"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
@@ -3472,7 +3468,7 @@
       <c r="J66" s="28"/>
       <c r="K66" s="39"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="19"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
@@ -3485,7 +3481,7 @@
       <c r="J67" s="28"/>
       <c r="K67" s="39"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="19"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
@@ -3498,7 +3494,7 @@
       <c r="J68" s="28"/>
       <c r="K68" s="39"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="19"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
@@ -3511,7 +3507,7 @@
       <c r="J69" s="28"/>
       <c r="K69" s="39"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="19"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
@@ -3524,7 +3520,7 @@
       <c r="J70" s="28"/>
       <c r="K70" s="39"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="19"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
@@ -3537,7 +3533,7 @@
       <c r="J71" s="28"/>
       <c r="K71" s="39"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="19"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
@@ -3550,7 +3546,7 @@
       <c r="J72" s="28"/>
       <c r="K72" s="39"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="19"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -3563,7 +3559,7 @@
       <c r="J73" s="28"/>
       <c r="K73" s="39"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="19"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
@@ -3576,7 +3572,7 @@
       <c r="J74" s="28"/>
       <c r="K74" s="39"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="19"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -3589,7 +3585,7 @@
       <c r="J75" s="28"/>
       <c r="K75" s="39"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="19"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -3602,7 +3598,7 @@
       <c r="J76" s="28"/>
       <c r="K76" s="39"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="19"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -3615,7 +3611,7 @@
       <c r="J77" s="28"/>
       <c r="K77" s="39"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="19"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -3628,7 +3624,7 @@
       <c r="J78" s="28"/>
       <c r="K78" s="39"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="19"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -3641,7 +3637,7 @@
       <c r="J79" s="28"/>
       <c r="K79" s="39"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="19"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -3654,7 +3650,7 @@
       <c r="J80" s="28"/>
       <c r="K80" s="39"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="19"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3667,7 +3663,7 @@
       <c r="J81" s="28"/>
       <c r="K81" s="39"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="19"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3680,7 +3676,7 @@
       <c r="J82" s="28"/>
       <c r="K82" s="39"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="19"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3693,7 +3689,7 @@
       <c r="J83" s="28"/>
       <c r="K83" s="39"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="19"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3706,7 +3702,7 @@
       <c r="J84" s="28"/>
       <c r="K84" s="39"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="19"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3719,7 +3715,7 @@
       <c r="J85" s="28"/>
       <c r="K85" s="39"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="19"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3732,7 +3728,7 @@
       <c r="J86" s="28"/>
       <c r="K86" s="39"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="19"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -3745,7 +3741,7 @@
       <c r="J87" s="28"/>
       <c r="K87" s="39"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="19"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -3758,7 +3754,7 @@
       <c r="J88" s="28"/>
       <c r="K88" s="39"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="19"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -3771,7 +3767,7 @@
       <c r="J89" s="28"/>
       <c r="K89" s="39"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="19"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -3784,7 +3780,7 @@
       <c r="J90" s="28"/>
       <c r="K90" s="39"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="19"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
@@ -3797,7 +3793,7 @@
       <c r="J91" s="28"/>
       <c r="K91" s="39"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="19"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
@@ -3810,7 +3806,7 @@
       <c r="J92" s="28"/>
       <c r="K92" s="39"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
@@ -3823,7 +3819,7 @@
       <c r="J93" s="28"/>
       <c r="K93" s="39"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="19"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
@@ -3836,7 +3832,7 @@
       <c r="J94" s="28"/>
       <c r="K94" s="39"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="19"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
@@ -3849,7 +3845,7 @@
       <c r="J95" s="28"/>
       <c r="K95" s="39"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="19"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
@@ -3862,7 +3858,7 @@
       <c r="J96" s="28"/>
       <c r="K96" s="39"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="19"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
@@ -3875,7 +3871,7 @@
       <c r="J97" s="28"/>
       <c r="K97" s="39"/>
     </row>
-    <row r="98" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
       <c r="B98" s="10"/>
       <c r="C98" s="11"/>
@@ -3912,7 +3908,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -3926,7 +3922,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>

<commit_message>
Úprava podle generátoru skutečnosti a výpočet EVy
</commit_message>
<xml_diff>
--- a/414_003_T02_PZp_priloha_B.xlsx
+++ b/414_003_T02_PZp_priloha_B.xlsx
@@ -1,27 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\Vysoka_skola\Magisterske_studium\2.ročník-ZS\4IT414-Rizeni_projektu\Semestralka\MS-Project-4IT414\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vse-my.sharepoint.com/personal/posm04_vse_cz/Documents/ZS2020/Řízení_projektů/MS Project REPO/MS-Project-4IT414/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C257E4-683B-4B14-A68F-019D29001946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{60181E14-34DB-4A46-A511-8E0CD0EC61F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -70,9 +74,6 @@
     <t>Zaokrouhlit střední hodnotu =</t>
   </si>
   <si>
-    <t>Ano</t>
-  </si>
-  <si>
     <t>Zaokrouhlení skut. doby trvání =</t>
   </si>
   <si>
@@ -236,6 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">   Otestování aplikace v produkčním prostředí čili kontrola, zda migrace proběhla v pořádku</t>
+  </si>
+  <si>
+    <t>Ne</t>
   </si>
 </sst>
 </file>
@@ -865,6 +869,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,13 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,55 +1234,55 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="K36" sqref="K4:K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="98.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="16" style="34" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="27" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="37.5703125" style="32" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" customWidth="1"/>
+    <col min="12" max="12" width="37.5546875" style="32" customWidth="1"/>
+    <col min="13" max="14" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="41" t="s">
+    <row r="1" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="49" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" s="33">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
@@ -1307,36 +1311,36 @@
         <v>7</v>
       </c>
       <c r="J3" s="31"/>
-      <c r="K3" s="47"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M3" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="49">
+      <c r="B4" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="42">
         <f>SUM(C5:C22)</f>
         <v>66</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="42">
         <f t="shared" ref="D4:E4" si="0">SUM(D5:D22)</f>
         <v>97</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="42">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="F4" s="1">
         <f>IF($M$4 = "Ano", ROUND((+E4+C4+4*D4)/6,0),(+E4+C4+4*D4)/6)</f>
-        <v>97</v>
+        <v>97.333333333333329</v>
       </c>
       <c r="G4" s="4">
         <f>+(E4-C4)/$M$2</f>
@@ -1344,37 +1348,37 @@
       </c>
       <c r="H4" s="23">
         <f ca="1">LN(_xlfn.LOGNORM.INV(RAND(),F4,G4))</f>
-        <v>77.149169649348678</v>
+        <v>76.509723715797449</v>
       </c>
       <c r="I4" s="35">
         <f ca="1">ROUND(IF(G4=0,F4,IF(H4&lt;F4,F4,H4)),$M$3)</f>
-        <v>97</v>
+        <v>97.33</v>
       </c>
       <c r="J4" s="30"/>
       <c r="K4" s="39">
-        <v>97</v>
+        <v>124.08</v>
       </c>
       <c r="L4" s="38" t="s">
         <v>12</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="50">
-        <v>2</v>
-      </c>
-      <c r="D5" s="50">
+      <c r="B5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="43">
+        <v>2</v>
+      </c>
+      <c r="D5" s="43">
         <v>3</v>
       </c>
-      <c r="E5" s="50">
+      <c r="E5" s="43">
         <v>4</v>
       </c>
       <c r="F5" s="1">
@@ -1387,31 +1391,31 @@
       </c>
       <c r="H5" s="23">
         <f t="shared" ref="H5:H58" ca="1" si="3">LN(_xlfn.LOGNORM.INV(RAND(),F5,G5))</f>
-        <v>2.5905777410561828</v>
+        <v>3.7426628550347862</v>
       </c>
       <c r="I5" s="35">
-        <f t="shared" ref="H5:K58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
-        <v>3</v>
+        <f t="shared" ref="I5:I58" ca="1" si="4">ROUND(IF(G5=0,F5,IF(H5&lt;F5,F5,H5)),$M$3)</f>
+        <v>3.74</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" s="39">
-        <v>4.1100000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="50">
-        <v>2</v>
-      </c>
-      <c r="D6" s="50">
+      <c r="B6" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="43">
+        <v>2</v>
+      </c>
+      <c r="D6" s="43">
         <v>3</v>
       </c>
-      <c r="E6" s="50">
+      <c r="E6" s="43">
         <v>4</v>
       </c>
       <c r="F6" s="1">
@@ -1424,31 +1428,31 @@
       </c>
       <c r="H6" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9114747343017386</v>
+        <v>3.2936499891988773</v>
       </c>
       <c r="I6" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.29</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="39">
-        <v>3.21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>4</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="50">
+      <c r="B7" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="43">
         <v>3</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="43">
         <v>4</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="43">
         <v>5</v>
       </c>
       <c r="F7" s="1">
@@ -1461,36 +1465,36 @@
       </c>
       <c r="H7" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0852352723457162</v>
+        <v>5.4077875160347038</v>
       </c>
       <c r="I7" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5.41</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="39">
-        <v>4.87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="50">
+      <c r="B8" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="43">
         <v>4</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="43">
         <v>5</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="43">
         <v>7</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="2"/>
@@ -1498,31 +1502,31 @@
       </c>
       <c r="H8" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.2021872523261656</v>
+        <v>5.2184012771051833</v>
       </c>
       <c r="I8" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.22</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>6</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="50">
-        <v>2</v>
-      </c>
-      <c r="D9" s="50">
+      <c r="B9" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="43">
+        <v>2</v>
+      </c>
+      <c r="D9" s="43">
         <v>3</v>
       </c>
-      <c r="E9" s="50">
+      <c r="E9" s="43">
         <v>4</v>
       </c>
       <c r="F9" s="1">
@@ -1535,7 +1539,7 @@
       </c>
       <c r="H9" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9257409550891769</v>
+        <v>2.5273301147350247</v>
       </c>
       <c r="I9" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1543,23 +1547,23 @@
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="39">
-        <v>3.18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>7</v>
       </c>
-      <c r="B10" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="50">
+      <c r="B10" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="43">
         <v>6</v>
       </c>
-      <c r="D10" s="50">
+      <c r="D10" s="43">
         <v>10</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="43">
         <v>14</v>
       </c>
       <c r="F10" s="1">
@@ -1572,36 +1576,36 @@
       </c>
       <c r="H10" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.718913771901137</v>
+        <v>11.586524418950049</v>
       </c>
       <c r="I10" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.72</v>
+        <v>11.59</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="39">
-        <v>12.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>11.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="50">
+      <c r="B11" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="43">
         <v>4</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D11" s="43">
         <v>5</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="43">
         <v>5</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="2"/>
@@ -1609,31 +1613,31 @@
       </c>
       <c r="H11" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.3853748854680283</v>
+        <v>4.5731996211992989</v>
       </c>
       <c r="I11" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.39</v>
+        <v>4.83</v>
       </c>
       <c r="J11" s="28"/>
       <c r="K11" s="39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="50">
+      <c r="B12" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="43">
         <v>1</v>
       </c>
-      <c r="D12" s="50">
-        <v>2</v>
-      </c>
-      <c r="E12" s="50">
+      <c r="D12" s="43">
+        <v>2</v>
+      </c>
+      <c r="E12" s="43">
         <v>3</v>
       </c>
       <c r="F12" s="1">
@@ -1646,7 +1650,7 @@
       </c>
       <c r="H12" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9828523474253772</v>
+        <v>1.8010068087242308</v>
       </c>
       <c r="I12" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1654,23 +1658,23 @@
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="50">
+      <c r="B13" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="43">
         <v>3</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="43">
         <v>4</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="43">
         <v>5</v>
       </c>
       <c r="F13" s="1">
@@ -1683,31 +1687,31 @@
       </c>
       <c r="H13" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1135753207259422</v>
+        <v>4.1361986515784093</v>
       </c>
       <c r="I13" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="39">
-        <v>4.51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="50">
-        <v>2</v>
-      </c>
-      <c r="D14" s="50">
+      <c r="B14" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="43">
+        <v>2</v>
+      </c>
+      <c r="D14" s="43">
         <v>3</v>
       </c>
-      <c r="E14" s="50">
+      <c r="E14" s="43">
         <v>4</v>
       </c>
       <c r="F14" s="1">
@@ -1720,36 +1724,36 @@
       </c>
       <c r="H14" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2176997360846005</v>
+        <v>2.7277181261835035</v>
       </c>
       <c r="I14" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.22</v>
+        <v>3</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="39">
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="50">
+      <c r="B15" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="43">
         <v>6</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="43">
         <v>8</v>
       </c>
-      <c r="E15" s="50">
+      <c r="E15" s="43">
         <v>11</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>8.1666666666666661</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="2"/>
@@ -1757,31 +1761,31 @@
       </c>
       <c r="H15" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5408511348571707</v>
+        <v>7.6612180290147442</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>8.17</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="39">
-        <v>9.26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8.17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="50">
+      <c r="B16" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="43">
         <v>4</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="43">
         <v>7</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="43">
         <v>10</v>
       </c>
       <c r="F16" s="1">
@@ -1794,31 +1798,31 @@
       </c>
       <c r="H16" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.5248715608404275</v>
+        <v>7.8158047537448923</v>
       </c>
       <c r="I16" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>7.82</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="50">
+      <c r="B17" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="43">
         <v>6</v>
       </c>
-      <c r="D17" s="50">
+      <c r="D17" s="43">
         <v>10</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="43">
         <v>14</v>
       </c>
       <c r="F17" s="1">
@@ -1831,31 +1835,31 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.316890041642326</v>
+        <v>9.4556784513624894</v>
       </c>
       <c r="I17" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.32</v>
+        <v>10</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>10.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="50">
+      <c r="B18" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="43">
         <v>3</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="43">
         <v>4</v>
       </c>
-      <c r="E18" s="50">
+      <c r="E18" s="43">
         <v>5</v>
       </c>
       <c r="F18" s="1">
@@ -1868,7 +1872,7 @@
       </c>
       <c r="H18" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7389870078287406</v>
+        <v>3.9837069238643923</v>
       </c>
       <c r="I18" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1876,28 +1880,28 @@
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="39">
-        <v>4.17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>16</v>
       </c>
-      <c r="B19" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="50">
+      <c r="B19" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="43">
         <v>6</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="43">
         <v>8</v>
       </c>
-      <c r="E19" s="50">
+      <c r="E19" s="43">
         <v>11</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>8.1666666666666661</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="2"/>
@@ -1905,31 +1909,31 @@
       </c>
       <c r="H19" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>10.234661405537191</v>
+        <v>6.9138964933889655</v>
       </c>
       <c r="I19" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10.23</v>
+        <v>8.17</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="39">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>17</v>
       </c>
-      <c r="B20" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="50">
+      <c r="B20" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="43">
         <v>6</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="43">
         <v>10</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="43">
         <v>14</v>
       </c>
       <c r="F20" s="1">
@@ -1942,7 +1946,7 @@
       </c>
       <c r="H20" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.0396488216739179</v>
+        <v>9.1723382113804419</v>
       </c>
       <c r="I20" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1950,23 +1954,23 @@
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="50">
+      <c r="B21" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="43">
         <v>3</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="43">
         <v>4</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="43">
         <v>5</v>
       </c>
       <c r="F21" s="1">
@@ -1979,7 +1983,7 @@
       </c>
       <c r="H21" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3813070765421367</v>
+        <v>3.9198494859400559</v>
       </c>
       <c r="I21" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -1987,23 +1991,23 @@
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="50">
+      <c r="B22" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="43">
         <v>3</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="43">
         <v>4</v>
       </c>
-      <c r="E22" s="50">
+      <c r="E22" s="43">
         <v>5</v>
       </c>
       <c r="F22" s="1">
@@ -2016,39 +2020,39 @@
       </c>
       <c r="H22" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.90184742779181</v>
+        <v>4.759144529114514</v>
       </c>
       <c r="I22" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>4.76</v>
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>20</v>
       </c>
-      <c r="B23" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="49">
+      <c r="B23" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="42">
         <f>SUM(C24:C34)</f>
         <v>15</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="42">
         <f t="shared" ref="D23:E23" si="5">SUM(D24:D34)</f>
         <v>26</v>
       </c>
-      <c r="E23" s="49">
+      <c r="E23" s="42">
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>26.833333333333332</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="2"/>
@@ -2056,31 +2060,31 @@
       </c>
       <c r="H23" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>27.821704307587016</v>
+        <v>34.384232500215454</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>27.82</v>
+        <v>34.380000000000003</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="39">
-        <v>27.59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>21</v>
       </c>
-      <c r="B24" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="50">
+      <c r="B24" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="43">
         <v>3</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="43">
         <v>4</v>
       </c>
-      <c r="E24" s="50">
+      <c r="E24" s="43">
         <v>5</v>
       </c>
       <c r="F24" s="1">
@@ -2093,31 +2097,31 @@
       </c>
       <c r="H24" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.8708828097095651</v>
+        <v>4.2496609401603509</v>
       </c>
       <c r="I24" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>4.87</v>
+        <v>4.25</v>
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>22</v>
       </c>
-      <c r="B25" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="50">
+      <c r="B25" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="43">
         <v>1</v>
       </c>
-      <c r="D25" s="50">
-        <v>2</v>
-      </c>
-      <c r="E25" s="50">
+      <c r="D25" s="43">
+        <v>2</v>
+      </c>
+      <c r="E25" s="43">
         <v>3</v>
       </c>
       <c r="F25" s="1">
@@ -2130,36 +2134,36 @@
       </c>
       <c r="H25" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.5580234517740843</v>
+        <v>2.1455544616110793</v>
       </c>
       <c r="I25" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.56</v>
+        <v>2.15</v>
       </c>
       <c r="J25" s="28"/>
       <c r="K25" s="39">
-        <v>2.86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>23</v>
       </c>
-      <c r="B26" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="50">
+      <c r="B26" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="43">
         <v>1</v>
       </c>
-      <c r="D26" s="50">
-        <v>2</v>
-      </c>
-      <c r="E26" s="50">
+      <c r="D26" s="43">
+        <v>2</v>
+      </c>
+      <c r="E26" s="43">
         <v>4</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="2"/>
@@ -2167,36 +2171,36 @@
       </c>
       <c r="H26" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.5699476409791187</v>
+        <v>3.0091692505926155</v>
       </c>
       <c r="I26" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3.01</v>
       </c>
       <c r="J26" s="28"/>
       <c r="K26" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>24</v>
       </c>
-      <c r="B27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="50">
+      <c r="B27" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="43">
         <v>1</v>
       </c>
-      <c r="D27" s="50">
-        <v>2</v>
-      </c>
-      <c r="E27" s="50">
+      <c r="D27" s="43">
+        <v>2</v>
+      </c>
+      <c r="E27" s="43">
         <v>4</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="2"/>
@@ -2204,31 +2208,31 @@
       </c>
       <c r="H27" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6482961409400545</v>
+        <v>2.9953345698006513</v>
       </c>
       <c r="I27" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.65</v>
+        <v>3</v>
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="39">
-        <v>2.39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>25</v>
       </c>
-      <c r="B28" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="50">
+      <c r="B28" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="43">
         <v>1</v>
       </c>
-      <c r="D28" s="50">
-        <v>2</v>
-      </c>
-      <c r="E28" s="50">
+      <c r="D28" s="43">
+        <v>2</v>
+      </c>
+      <c r="E28" s="43">
         <v>3</v>
       </c>
       <c r="F28" s="1">
@@ -2241,31 +2245,31 @@
       </c>
       <c r="H28" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9132933285596767</v>
+        <v>2.0577378395235004</v>
       </c>
       <c r="I28" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.06</v>
       </c>
       <c r="J28" s="28"/>
       <c r="K28" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>26</v>
       </c>
-      <c r="B29" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="50">
+      <c r="B29" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="43">
         <v>3</v>
       </c>
-      <c r="D29" s="50">
+      <c r="D29" s="43">
         <v>4</v>
       </c>
-      <c r="E29" s="50">
+      <c r="E29" s="43">
         <v>5</v>
       </c>
       <c r="F29" s="1">
@@ -2278,7 +2282,7 @@
       </c>
       <c r="H29" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.8243691773235975</v>
+        <v>3.97255792263095</v>
       </c>
       <c r="I29" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2286,28 +2290,28 @@
       </c>
       <c r="J29" s="28"/>
       <c r="K29" s="39">
-        <v>4.6399999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>27</v>
       </c>
-      <c r="B30" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="50">
+      <c r="B30" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="43">
         <v>1</v>
       </c>
-      <c r="D30" s="50">
-        <v>2</v>
-      </c>
-      <c r="E30" s="50">
+      <c r="D30" s="43">
+        <v>2</v>
+      </c>
+      <c r="E30" s="43">
         <v>4</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="2"/>
@@ -2315,36 +2319,36 @@
       </c>
       <c r="H30" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.0345954232236316</v>
+        <v>0.79820094511172535</v>
       </c>
       <c r="I30" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.0299999999999998</v>
+        <v>2.17</v>
       </c>
       <c r="J30" s="28"/>
       <c r="K30" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>28</v>
       </c>
-      <c r="B31" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="50">
+      <c r="B31" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="43">
         <v>1</v>
       </c>
-      <c r="D31" s="50">
-        <v>2</v>
-      </c>
-      <c r="E31" s="50">
+      <c r="D31" s="43">
+        <v>2</v>
+      </c>
+      <c r="E31" s="43">
         <v>4</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="2"/>
@@ -2352,36 +2356,36 @@
       </c>
       <c r="H31" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1385546758098797</v>
+        <v>1.9510564804768074</v>
       </c>
       <c r="I31" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>2.17</v>
       </c>
       <c r="J31" s="28"/>
       <c r="K31" s="39">
-        <v>3.09</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>29</v>
       </c>
-      <c r="B32" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="50">
+      <c r="B32" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="43">
         <v>1</v>
       </c>
-      <c r="D32" s="50">
-        <v>2</v>
-      </c>
-      <c r="E32" s="50">
+      <c r="D32" s="43">
+        <v>2</v>
+      </c>
+      <c r="E32" s="43">
         <v>4</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.1666666666666665</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="2"/>
@@ -2389,31 +2393,31 @@
       </c>
       <c r="H32" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.93345268338986931</v>
+        <v>3.3535974985127917</v>
       </c>
       <c r="I32" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3.35</v>
       </c>
       <c r="J32" s="28"/>
       <c r="K32" s="39">
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>30</v>
       </c>
-      <c r="B33" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="50">
+      <c r="B33" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="43">
         <v>1</v>
       </c>
-      <c r="D33" s="50">
-        <v>2</v>
-      </c>
-      <c r="E33" s="50">
+      <c r="D33" s="43">
+        <v>2</v>
+      </c>
+      <c r="E33" s="43">
         <v>3</v>
       </c>
       <c r="F33" s="1">
@@ -2426,31 +2430,31 @@
       </c>
       <c r="H33" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.8509747188136898</v>
+        <v>1.5237868066532985</v>
       </c>
       <c r="I33" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.85</v>
+        <v>2</v>
       </c>
       <c r="J33" s="28"/>
       <c r="K33" s="39">
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>31</v>
       </c>
-      <c r="B34" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="50">
+      <c r="B34" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="43">
         <v>1</v>
       </c>
-      <c r="D34" s="50">
-        <v>2</v>
-      </c>
-      <c r="E34" s="50">
+      <c r="D34" s="43">
+        <v>2</v>
+      </c>
+      <c r="E34" s="43">
         <v>3</v>
       </c>
       <c r="F34" s="1">
@@ -2463,39 +2467,39 @@
       </c>
       <c r="H34" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.0286524274824602</v>
+        <v>1.7607883693930548</v>
       </c>
       <c r="I34" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.03</v>
+        <v>2</v>
       </c>
       <c r="J34" s="28"/>
       <c r="K34" s="39">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>32</v>
       </c>
-      <c r="B35" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="49">
+      <c r="B35" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="42">
         <f>SUM(C36:C51)</f>
         <v>77</v>
       </c>
-      <c r="D35" s="49">
+      <c r="D35" s="42">
         <f t="shared" ref="D35:E35" si="6">SUM(D36:D51)</f>
         <v>152</v>
       </c>
-      <c r="E35" s="49">
+      <c r="E35" s="42">
         <f t="shared" si="6"/>
         <v>235</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="1"/>
-        <v>153</v>
+        <v>153.33333333333334</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="2"/>
@@ -2503,36 +2507,36 @@
       </c>
       <c r="H35" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>170.19109632569635</v>
+        <v>214.22082871643877</v>
       </c>
       <c r="I35" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>170.19</v>
+        <v>214.22</v>
       </c>
       <c r="J35" s="28"/>
       <c r="K35" s="39">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>153.33000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>33</v>
       </c>
-      <c r="B36" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="50">
+      <c r="B36" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="43">
         <v>3</v>
       </c>
-      <c r="D36" s="50">
+      <c r="D36" s="43">
         <v>5</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="43">
         <v>8</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="2"/>
@@ -2540,36 +2544,36 @@
       </c>
       <c r="H36" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.1500762632544772</v>
+        <v>5.2645977185457911</v>
       </c>
       <c r="I36" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.26</v>
       </c>
       <c r="J36" s="28"/>
       <c r="K36" s="39">
-        <v>5.21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>34</v>
       </c>
-      <c r="B37" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="50">
+      <c r="B37" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="43">
         <v>3</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="43">
         <v>6</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="43">
         <v>10</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="2"/>
@@ -2577,31 +2581,31 @@
       </c>
       <c r="H37" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>6.1191999240944099</v>
+        <v>5.5322520377265167</v>
       </c>
       <c r="I37" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>6.12</v>
+        <v>6.17</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="39">
-        <v>7.17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>35</v>
       </c>
-      <c r="B38" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="50">
+      <c r="B38" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="43">
         <v>15</v>
       </c>
-      <c r="D38" s="50">
+      <c r="D38" s="43">
         <v>35</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="43">
         <v>55</v>
       </c>
       <c r="F38" s="1">
@@ -2614,36 +2618,36 @@
       </c>
       <c r="H38" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>59.434880607771674</v>
+        <v>19.90928904715426</v>
       </c>
       <c r="I38" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>59.43</v>
+        <v>35</v>
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="39">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>45.09</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>36</v>
       </c>
-      <c r="B39" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="50">
+      <c r="B39" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="43">
         <v>3</v>
       </c>
-      <c r="D39" s="50">
+      <c r="D39" s="43">
         <v>5</v>
       </c>
-      <c r="E39" s="50">
+      <c r="E39" s="43">
         <v>8</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="2"/>
@@ -2651,36 +2655,36 @@
       </c>
       <c r="H39" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7421726032849261</v>
+        <v>5.5987209295923837</v>
       </c>
       <c r="I39" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5.74</v>
+        <v>5.6</v>
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="39">
-        <v>6.09</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>37</v>
       </c>
-      <c r="B40" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="50">
+      <c r="B40" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="43">
         <v>6</v>
       </c>
-      <c r="D40" s="50">
+      <c r="D40" s="43">
         <v>9</v>
       </c>
-      <c r="E40" s="50">
+      <c r="E40" s="43">
         <v>15</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="2"/>
@@ -2688,31 +2692,31 @@
       </c>
       <c r="H40" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.5810969944735369</v>
+        <v>9.883000807925038</v>
       </c>
       <c r="I40" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9.8800000000000008</v>
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>38</v>
       </c>
-      <c r="B41" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="50">
-        <v>2</v>
-      </c>
-      <c r="D41" s="50">
+      <c r="B41" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="43">
+        <v>2</v>
+      </c>
+      <c r="D41" s="43">
         <v>5</v>
       </c>
-      <c r="E41" s="50">
+      <c r="E41" s="43">
         <v>8</v>
       </c>
       <c r="F41" s="1">
@@ -2725,36 +2729,36 @@
       </c>
       <c r="H41" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.7221699751293684</v>
+        <v>4.6344589709969837</v>
       </c>
       <c r="I41" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>7.72</v>
+        <v>5</v>
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>39</v>
       </c>
-      <c r="B42" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="50">
-        <v>2</v>
-      </c>
-      <c r="D42" s="50">
+      <c r="B42" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="43">
+        <v>2</v>
+      </c>
+      <c r="D42" s="43">
         <v>3</v>
       </c>
-      <c r="E42" s="50">
+      <c r="E42" s="43">
         <v>5</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="2"/>
@@ -2762,36 +2766,36 @@
       </c>
       <c r="H42" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.6607536012778636</v>
+        <v>2.6193435635461153</v>
       </c>
       <c r="I42" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>3.17</v>
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="39">
-        <v>3.16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>40</v>
       </c>
-      <c r="B43" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="50">
+      <c r="B43" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="43">
         <v>3</v>
       </c>
-      <c r="D43" s="50">
+      <c r="D43" s="43">
         <v>6</v>
       </c>
-      <c r="E43" s="50">
+      <c r="E43" s="43">
         <v>8</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="2"/>
@@ -2799,31 +2803,31 @@
       </c>
       <c r="H43" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>8.6320491664757029</v>
+        <v>5.8190106570731173</v>
       </c>
       <c r="I43" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>8.6300000000000008</v>
+        <v>5.83</v>
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="39">
-        <v>7.33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>41</v>
       </c>
-      <c r="B44" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="50">
+      <c r="B44" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="43">
         <v>10</v>
       </c>
-      <c r="D44" s="50">
+      <c r="D44" s="43">
         <v>20</v>
       </c>
-      <c r="E44" s="50">
+      <c r="E44" s="43">
         <v>30</v>
       </c>
       <c r="F44" s="1">
@@ -2836,7 +2840,7 @@
       </c>
       <c r="H44" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>13.630711908261214</v>
+        <v>16.009796493671097</v>
       </c>
       <c r="I44" s="35">
         <f t="shared" ca="1" si="4"/>
@@ -2847,20 +2851,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>42</v>
       </c>
-      <c r="B45" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="50">
+      <c r="B45" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="43">
         <v>5</v>
       </c>
-      <c r="D45" s="50">
+      <c r="D45" s="43">
         <v>10</v>
       </c>
-      <c r="E45" s="50">
+      <c r="E45" s="43">
         <v>15</v>
       </c>
       <c r="F45" s="1">
@@ -2873,31 +2877,31 @@
       </c>
       <c r="H45" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>11.302629898425314</v>
+        <v>8.1780469388101587</v>
       </c>
       <c r="I45" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>11.3</v>
+        <v>10</v>
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="39">
-        <v>10.050000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>43</v>
       </c>
-      <c r="B46" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="50">
+      <c r="B46" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="43">
         <v>10</v>
       </c>
-      <c r="D46" s="50">
+      <c r="D46" s="43">
         <v>20</v>
       </c>
-      <c r="E46" s="50">
+      <c r="E46" s="43">
         <v>30</v>
       </c>
       <c r="F46" s="1">
@@ -2910,36 +2914,36 @@
       </c>
       <c r="H46" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>19.921031266705697</v>
+        <v>22.795919520790278</v>
       </c>
       <c r="I46" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>20</v>
+        <v>22.8</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="39">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>22.31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>44</v>
       </c>
-      <c r="B47" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="50">
+      <c r="B47" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="43">
         <v>3</v>
       </c>
-      <c r="D47" s="50">
+      <c r="D47" s="43">
         <v>5</v>
       </c>
-      <c r="E47" s="50">
+      <c r="E47" s="43">
         <v>8</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="2"/>
@@ -2947,31 +2951,31 @@
       </c>
       <c r="H47" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.902438453875118</v>
+        <v>4.0034898102589924</v>
       </c>
       <c r="I47" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>5.17</v>
       </c>
       <c r="J47" s="28"/>
       <c r="K47" s="39">
-        <v>5.14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>45</v>
       </c>
-      <c r="B48" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="50">
+      <c r="B48" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="43">
         <v>1</v>
       </c>
-      <c r="D48" s="50">
-        <v>2</v>
-      </c>
-      <c r="E48" s="50">
+      <c r="D48" s="43">
+        <v>2</v>
+      </c>
+      <c r="E48" s="43">
         <v>3</v>
       </c>
       <c r="F48" s="1">
@@ -2984,36 +2988,36 @@
       </c>
       <c r="H48" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.3271163610881564</v>
+        <v>1.4911955989377619</v>
       </c>
       <c r="I48" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="39">
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>46</v>
       </c>
-      <c r="B49" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="50">
+      <c r="B49" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="43">
         <v>1</v>
       </c>
-      <c r="D49" s="50">
+      <c r="D49" s="43">
         <v>1</v>
       </c>
-      <c r="E49" s="50">
+      <c r="E49" s="43">
         <v>2</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="2"/>
@@ -3021,31 +3025,31 @@
       </c>
       <c r="H49" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6782906190755108</v>
+        <v>1.2256743754285364</v>
       </c>
       <c r="I49" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1.23</v>
       </c>
       <c r="J49" s="28"/>
       <c r="K49" s="39">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>47</v>
       </c>
-      <c r="B50" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="50">
+      <c r="B50" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="43">
         <v>5</v>
       </c>
-      <c r="D50" s="50">
+      <c r="D50" s="43">
         <v>10</v>
       </c>
-      <c r="E50" s="50">
+      <c r="E50" s="43">
         <v>15</v>
       </c>
       <c r="F50" s="1">
@@ -3058,31 +3062,31 @@
       </c>
       <c r="H50" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>7.0796816318331253</v>
+        <v>12.745222303711877</v>
       </c>
       <c r="I50" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>12.75</v>
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>48</v>
       </c>
-      <c r="B51" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="50">
+      <c r="B51" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="43">
         <v>5</v>
       </c>
-      <c r="D51" s="50">
+      <c r="D51" s="43">
         <v>10</v>
       </c>
-      <c r="E51" s="50">
+      <c r="E51" s="43">
         <v>15</v>
       </c>
       <c r="F51" s="1">
@@ -3095,39 +3099,39 @@
       </c>
       <c r="H51" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>9.9873873171284639</v>
+        <v>14.149524913779789</v>
       </c>
       <c r="I51" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>14.15</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="39">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>49</v>
       </c>
-      <c r="B52" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="49">
+      <c r="B52" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="42">
         <f>SUM(C53:C58)</f>
         <v>21</v>
       </c>
-      <c r="D52" s="49">
+      <c r="D52" s="42">
         <f t="shared" ref="D52:E52" si="7">SUM(D53:D58)</f>
         <v>29</v>
       </c>
-      <c r="E52" s="49">
+      <c r="E52" s="42">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29.5</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="2"/>
@@ -3135,36 +3139,36 @@
       </c>
       <c r="H52" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>33.341819154237271</v>
+        <v>28.689093743737278</v>
       </c>
       <c r="I52" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>33.340000000000003</v>
+        <v>29.5</v>
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="39">
-        <v>34.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34.479999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>50</v>
       </c>
-      <c r="B53" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="50">
-        <v>2</v>
-      </c>
-      <c r="D53" s="50">
+      <c r="B53" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="43">
+        <v>2</v>
+      </c>
+      <c r="D53" s="43">
         <v>3</v>
       </c>
-      <c r="E53" s="50">
+      <c r="E53" s="43">
         <v>5</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" si="2"/>
@@ -3172,36 +3176,36 @@
       </c>
       <c r="H53" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.1158791945389992</v>
+        <v>2.5920160706323694</v>
       </c>
       <c r="I53" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.12</v>
+        <v>3.17</v>
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="39">
-        <v>4.1500000000000004</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>51</v>
       </c>
-      <c r="B54" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="50">
+      <c r="B54" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="43">
         <v>1</v>
       </c>
-      <c r="D54" s="50">
+      <c r="D54" s="43">
         <v>1</v>
       </c>
-      <c r="E54" s="50">
+      <c r="E54" s="43">
         <v>2</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="G54" s="4">
         <f t="shared" si="2"/>
@@ -3209,31 +3213,31 @@
       </c>
       <c r="H54" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>0.77707082826872553</v>
+        <v>1.1216815618064473</v>
       </c>
       <c r="I54" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1.17</v>
       </c>
       <c r="J54" s="28"/>
       <c r="K54" s="39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>52</v>
       </c>
-      <c r="B55" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="50">
+      <c r="B55" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="43">
         <v>1</v>
       </c>
-      <c r="D55" s="50">
-        <v>2</v>
-      </c>
-      <c r="E55" s="50">
+      <c r="D55" s="43">
+        <v>2</v>
+      </c>
+      <c r="E55" s="43">
         <v>3</v>
       </c>
       <c r="F55" s="1">
@@ -3246,36 +3250,36 @@
       </c>
       <c r="H55" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>2.1056702636022044</v>
+        <v>1.7926198376510052</v>
       </c>
       <c r="I55" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>2.11</v>
+        <v>2</v>
       </c>
       <c r="J55" s="28"/>
       <c r="K55" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>53</v>
       </c>
-      <c r="B56" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="50">
+      <c r="B56" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="43">
         <v>12</v>
       </c>
-      <c r="D56" s="50">
+      <c r="D56" s="43">
         <v>15</v>
       </c>
-      <c r="E56" s="50">
+      <c r="E56" s="43">
         <v>17</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14.833333333333334</v>
       </c>
       <c r="G56" s="4">
         <f t="shared" si="2"/>
@@ -3283,36 +3287,36 @@
       </c>
       <c r="H56" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>14.541766659713996</v>
+        <v>14.615164786231574</v>
       </c>
       <c r="I56" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>15</v>
+        <v>14.83</v>
       </c>
       <c r="J56" s="28"/>
       <c r="K56" s="39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>14.83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>54</v>
       </c>
-      <c r="B57" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="C57" s="50">
+      <c r="B57" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="43">
         <v>3</v>
       </c>
-      <c r="D57" s="50">
+      <c r="D57" s="43">
         <v>5</v>
       </c>
-      <c r="E57" s="50">
+      <c r="E57" s="43">
         <v>8</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="G57" s="4">
         <f t="shared" si="2"/>
@@ -3320,36 +3324,36 @@
       </c>
       <c r="H57" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>4.3248421810813156</v>
+        <v>6.6798026046617647</v>
       </c>
       <c r="I57" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>6.68</v>
       </c>
       <c r="J57" s="28"/>
       <c r="K57" s="39">
-        <v>7.27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>55</v>
       </c>
-      <c r="B58" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="50">
-        <v>2</v>
-      </c>
-      <c r="D58" s="50">
+      <c r="B58" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="43">
+        <v>2</v>
+      </c>
+      <c r="D58" s="43">
         <v>3</v>
       </c>
-      <c r="E58" s="50">
+      <c r="E58" s="43">
         <v>5</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="2"/>
@@ -3357,18 +3361,18 @@
       </c>
       <c r="H58" s="23">
         <f t="shared" ca="1" si="3"/>
-        <v>3.3184840739195023</v>
+        <v>3.400120286267438</v>
       </c>
       <c r="I58" s="35">
         <f t="shared" ca="1" si="4"/>
-        <v>3.32</v>
+        <v>3.4</v>
       </c>
       <c r="J58" s="28"/>
       <c r="K58" s="39">
-        <v>3.97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="F59" s="2"/>
       <c r="G59" s="5"/>
@@ -3377,7 +3381,7 @@
       <c r="J59" s="28"/>
       <c r="K59" s="39"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
@@ -3390,7 +3394,7 @@
       <c r="J60" s="28"/>
       <c r="K60" s="39"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
@@ -3403,7 +3407,7 @@
       <c r="J61" s="28"/>
       <c r="K61" s="39"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
@@ -3416,7 +3420,7 @@
       <c r="J62" s="28"/>
       <c r="K62" s="39"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8"/>
@@ -3429,7 +3433,7 @@
       <c r="J63" s="28"/>
       <c r="K63" s="39"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
@@ -3442,7 +3446,7 @@
       <c r="J64" s="28"/>
       <c r="K64" s="39"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
@@ -3455,7 +3459,7 @@
       <c r="J65" s="28"/>
       <c r="K65" s="39"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
@@ -3468,7 +3472,7 @@
       <c r="J66" s="28"/>
       <c r="K66" s="39"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
@@ -3481,7 +3485,7 @@
       <c r="J67" s="28"/>
       <c r="K67" s="39"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
@@ -3494,7 +3498,7 @@
       <c r="J68" s="28"/>
       <c r="K68" s="39"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="7"/>
       <c r="C69" s="8"/>
@@ -3507,7 +3511,7 @@
       <c r="J69" s="28"/>
       <c r="K69" s="39"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
@@ -3520,7 +3524,7 @@
       <c r="J70" s="28"/>
       <c r="K70" s="39"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
@@ -3533,7 +3537,7 @@
       <c r="J71" s="28"/>
       <c r="K71" s="39"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="19"/>
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
@@ -3546,7 +3550,7 @@
       <c r="J72" s="28"/>
       <c r="K72" s="39"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="7"/>
       <c r="C73" s="8"/>
@@ -3559,7 +3563,7 @@
       <c r="J73" s="28"/>
       <c r="K73" s="39"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
@@ -3572,7 +3576,7 @@
       <c r="J74" s="28"/>
       <c r="K74" s="39"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -3585,7 +3589,7 @@
       <c r="J75" s="28"/>
       <c r="K75" s="39"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -3598,7 +3602,7 @@
       <c r="J76" s="28"/>
       <c r="K76" s="39"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -3611,7 +3615,7 @@
       <c r="J77" s="28"/>
       <c r="K77" s="39"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -3624,7 +3628,7 @@
       <c r="J78" s="28"/>
       <c r="K78" s="39"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -3637,7 +3641,7 @@
       <c r="J79" s="28"/>
       <c r="K79" s="39"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -3650,7 +3654,7 @@
       <c r="J80" s="28"/>
       <c r="K80" s="39"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3663,7 +3667,7 @@
       <c r="J81" s="28"/>
       <c r="K81" s="39"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3676,7 +3680,7 @@
       <c r="J82" s="28"/>
       <c r="K82" s="39"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3689,7 +3693,7 @@
       <c r="J83" s="28"/>
       <c r="K83" s="39"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3702,7 +3706,7 @@
       <c r="J84" s="28"/>
       <c r="K84" s="39"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="19"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8"/>
@@ -3715,7 +3719,7 @@
       <c r="J85" s="28"/>
       <c r="K85" s="39"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="19"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
@@ -3728,7 +3732,7 @@
       <c r="J86" s="28"/>
       <c r="K86" s="39"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="19"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
@@ -3741,7 +3745,7 @@
       <c r="J87" s="28"/>
       <c r="K87" s="39"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19"/>
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
@@ -3754,7 +3758,7 @@
       <c r="J88" s="28"/>
       <c r="K88" s="39"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="19"/>
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
@@ -3767,7 +3771,7 @@
       <c r="J89" s="28"/>
       <c r="K89" s="39"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="19"/>
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
@@ -3780,7 +3784,7 @@
       <c r="J90" s="28"/>
       <c r="K90" s="39"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="19"/>
       <c r="B91" s="7"/>
       <c r="C91" s="8"/>
@@ -3793,7 +3797,7 @@
       <c r="J91" s="28"/>
       <c r="K91" s="39"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="19"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
@@ -3806,7 +3810,7 @@
       <c r="J92" s="28"/>
       <c r="K92" s="39"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="19"/>
       <c r="B93" s="7"/>
       <c r="C93" s="8"/>
@@ -3819,7 +3823,7 @@
       <c r="J93" s="28"/>
       <c r="K93" s="39"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="19"/>
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
@@ -3832,7 +3836,7 @@
       <c r="J94" s="28"/>
       <c r="K94" s="39"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="19"/>
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
@@ -3845,7 +3849,7 @@
       <c r="J95" s="28"/>
       <c r="K95" s="39"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="19"/>
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
@@ -3858,7 +3862,7 @@
       <c r="J96" s="28"/>
       <c r="K96" s="39"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="19"/>
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
@@ -3871,7 +3875,7 @@
       <c r="J97" s="28"/>
       <c r="K97" s="39"/>
     </row>
-    <row r="98" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="10"/>
       <c r="C98" s="11"/>
@@ -3908,7 +3912,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -3922,7 +3926,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>